<commit_message>
feat: add random select
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3E76D5-48D6-4F4A-A252-AEC220D3E8E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76CE233-27E4-42CB-8267-B5BB34B66813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:E546"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1854,15 +1854,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>22210</v>
+        <v>22722</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>8.9044747959476644E-2</v>
+        <v>6.8044788975021531E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>6.4389041390994856E-2</v>
+        <v>3.4776403507067184E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>21687</v>
+        <v>22420</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>0.10657493614567026</v>
+        <v>7.6378017632034279E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1888,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>20914</v>
+        <v>21798</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>0.11196976773810029</v>
+        <v>7.4434206615430348E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1903,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>22693</v>
+        <v>23354</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>3.5735531571343591E-2</v>
+        <v>7.6485085408345369E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1918,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>22123</v>
+        <v>22496</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>7.7862531782751862E-2</v>
+        <v>6.2315034804718436E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,11 +1933,11 @@
         <v>24613</v>
       </c>
       <c r="C7" s="1">
-        <v>24136</v>
+        <v>24755</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>1.9380002437736157E-2</v>
+        <v>-5.7693089017998621E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>23416</v>
+        <v>24652</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>8.4990817084131143E-2</v>
+        <v>3.6692587237700754E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1963,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>21579</v>
+        <v>22557</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>7.8214438274241779E-2</v>
+        <v>3.6437419906023068E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1978,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>22786</v>
+        <v>22540</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>5.9051866534522629E-2</v>
+        <v>6.921043937892303E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1993,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>21094</v>
+        <v>23098</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>0.13588136495842038</v>
+        <v>5.3787227069763632E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2008,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>41131</v>
+        <v>42474</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>3.8028860771335687E-2</v>
+        <v>6.6187992609397289E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2023,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>39239</v>
+        <v>39563</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>7.7705958396991417E-2</v>
+        <v>7.0090492419790804E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2038,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>38724</v>
+        <v>39885</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>7.7296988181471599E-2</v>
+        <v>4.9633053755242088E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2053,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>39982</v>
+        <v>41232</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>0.113284542027057</v>
+        <v>8.5562208915502327E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2068,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>38430</v>
+        <v>39794</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>8.9724761949879203E-2</v>
+        <v>5.7416267942583733E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2083,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>37279</v>
+        <v>39636</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>0.13157220397418873</v>
+        <v>7.6665035991334132E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2098,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>38097</v>
+        <v>41000</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>9.3122902235235311E-2</v>
+        <v>2.4018662667523626E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2113,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>41040</v>
+        <v>41726</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>8.8405153265215461E-2</v>
+        <v>7.3167481119502442E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2128,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>39635</v>
+        <v>41940</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>8.7613084413342229E-2</v>
+        <v>3.4552611588131027E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2143,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>40092</v>
+        <v>43110</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>0.10014813484760067</v>
+        <v>3.2410109081115052E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2158,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>58098</v>
+        <v>58930</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>2.8818829193273377E-2</v>
+        <v>1.4910902343619404E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>60780</v>
+        <v>62089</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>2.0956492324543743E-2</v>
+        <v>-1.2886390360980011E-4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2188,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>57424</v>
+        <v>58918</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>3.9764556369352194E-2</v>
+        <v>1.4782114310558175E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2203,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>59345</v>
+        <v>60260</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>1.8750310024967343E-2</v>
+        <v>3.6210916185783495E-3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2218,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>57973</v>
+        <v>60604</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>5.1038614525871238E-2</v>
+        <v>7.9717143278060596E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2233,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>57674</v>
+        <v>58526</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>2.1794806560491188E-2</v>
+        <v>7.3440865686324394E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2248,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>60675</v>
+        <v>61853</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>1.4023855178913842E-2</v>
+        <v>-5.1187883909129322E-3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2263,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>60720</v>
+        <v>60675</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>1.3003901170351105E-2</v>
+        <v>1.3735370611183354E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2278,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>58675</v>
+        <v>59597</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>1.3085967066422215E-2</v>
+        <v>-2.4220813079239064E-3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>59076</v>
+        <v>60008</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>1.4825314766947387E-2</v>
+        <v>-7.1708496623030106E-4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2307,12 +2307,9 @@
       <c r="B32" s="1">
         <v>59312</v>
       </c>
-      <c r="C32" s="1">
-        <v>51970</v>
-      </c>
       <c r="D32" s="2">
         <f t="shared" si="0"/>
-        <v>0.12378608038845428</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2322,12 +2319,9 @@
       <c r="B33" s="1">
         <v>61472</v>
       </c>
-      <c r="C33" s="1">
-        <v>52972</v>
-      </c>
       <c r="D33" s="2">
         <f t="shared" si="0"/>
-        <v>0.13827433628318583</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -2337,12 +2331,9 @@
       <c r="B34" s="1">
         <v>62130</v>
       </c>
-      <c r="C34" s="1">
-        <v>52963</v>
-      </c>
       <c r="D34" s="2">
         <f t="shared" si="0"/>
-        <v>0.14754546917753097</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -2352,12 +2343,9 @@
       <c r="B35" s="1">
         <v>59446</v>
       </c>
-      <c r="C35" s="1">
-        <v>51547</v>
-      </c>
       <c r="D35" s="2">
         <f t="shared" si="0"/>
-        <v>0.13287689667933925</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -2367,12 +2355,9 @@
       <c r="B36" s="1">
         <v>58951</v>
       </c>
-      <c r="C36" s="1">
-        <v>52129</v>
-      </c>
       <c r="D36" s="2">
         <f t="shared" si="0"/>
-        <v>0.11572322776543231</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -2382,12 +2367,9 @@
       <c r="B37" s="1">
         <v>60056</v>
       </c>
-      <c r="C37" s="1">
-        <v>52746</v>
-      </c>
       <c r="D37" s="2">
         <f t="shared" si="0"/>
-        <v>0.12171972825362995</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2397,12 +2379,9 @@
       <c r="B38" s="1">
         <v>60414</v>
       </c>
-      <c r="C38" s="1">
-        <v>52576</v>
-      </c>
       <c r="D38" s="2">
         <f t="shared" si="0"/>
-        <v>0.12973814016618665</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2412,12 +2391,9 @@
       <c r="B39" s="1">
         <v>61472</v>
       </c>
-      <c r="C39" s="1">
-        <v>56204</v>
-      </c>
       <c r="D39" s="2">
         <f t="shared" si="0"/>
-        <v>8.569755335762623E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2427,12 +2403,9 @@
       <c r="B40" s="1">
         <v>61885</v>
       </c>
-      <c r="C40" s="1">
-        <v>52466</v>
-      </c>
       <c r="D40" s="2">
         <f t="shared" si="0"/>
-        <v>0.15220166437747434</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2442,12 +2415,9 @@
       <c r="B41" s="1">
         <v>58959</v>
       </c>
-      <c r="C41" s="1">
-        <v>51846</v>
-      </c>
       <c r="D41" s="2">
         <f t="shared" si="0"/>
-        <v>0.12064315880527146</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2457,12 +2427,9 @@
       <c r="B42" s="1">
         <v>109109</v>
       </c>
-      <c r="C42" s="1">
-        <v>96614</v>
-      </c>
       <c r="D42" s="2">
         <f t="shared" si="0"/>
-        <v>0.11451850901392185</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2472,12 +2439,9 @@
       <c r="B43" s="1">
         <v>109841</v>
       </c>
-      <c r="C43" s="1">
-        <v>95129</v>
-      </c>
       <c r="D43" s="2">
         <f t="shared" si="0"/>
-        <v>0.1339390573647363</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -2487,12 +2451,9 @@
       <c r="B44" s="1">
         <v>108489</v>
       </c>
-      <c r="C44" s="1">
-        <v>93832</v>
-      </c>
       <c r="D44" s="2">
         <f t="shared" si="0"/>
-        <v>0.13510125450506502</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2502,12 +2463,9 @@
       <c r="B45" s="1">
         <v>109383</v>
       </c>
-      <c r="C45" s="1">
-        <v>96864</v>
-      </c>
       <c r="D45" s="2">
         <f t="shared" si="0"/>
-        <v>0.11445105729409506</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2517,12 +2475,9 @@
       <c r="B46" s="1">
         <v>110720</v>
       </c>
-      <c r="C46" s="1">
-        <v>98073</v>
-      </c>
       <c r="D46" s="2">
         <f t="shared" si="0"/>
-        <v>0.11422507225433526</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2532,12 +2487,9 @@
       <c r="B47" s="1">
         <v>110256</v>
       </c>
-      <c r="C47" s="1">
-        <v>97273</v>
-      </c>
       <c r="D47" s="2">
         <f t="shared" si="0"/>
-        <v>0.11775322884922362</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2547,12 +2499,9 @@
       <c r="B48" s="1">
         <v>109016</v>
       </c>
-      <c r="C48" s="1">
-        <v>95917</v>
-      </c>
       <c r="D48" s="2">
         <f t="shared" si="0"/>
-        <v>0.12015667424965143</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2562,12 +2511,9 @@
       <c r="B49" s="1">
         <v>109037</v>
       </c>
-      <c r="C49" s="1">
-        <v>96792</v>
-      </c>
       <c r="D49" s="2">
         <f t="shared" si="0"/>
-        <v>0.1123013289067014</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2577,12 +2523,9 @@
       <c r="B50" s="1">
         <v>109957</v>
       </c>
-      <c r="C50" s="1">
-        <v>97105</v>
-      </c>
       <c r="D50" s="2">
         <f t="shared" si="0"/>
-        <v>0.11688205389379484</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2592,12 +2535,9 @@
       <c r="B51" s="1">
         <v>107038</v>
       </c>
-      <c r="C51" s="1">
-        <v>93349</v>
-      </c>
       <c r="D51" s="2">
         <f t="shared" si="0"/>
-        <v>0.12788916085876045</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2607,12 +2547,9 @@
       <c r="B52" s="1">
         <v>149659</v>
       </c>
-      <c r="C52" s="1">
-        <v>145771</v>
-      </c>
       <c r="D52" s="2">
         <f t="shared" si="0"/>
-        <v>2.5979059060931852E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2622,12 +2559,9 @@
       <c r="B53" s="1">
         <v>155940</v>
       </c>
-      <c r="C53" s="1">
-        <v>148608</v>
-      </c>
       <c r="D53" s="2">
         <f t="shared" si="0"/>
-        <v>4.7018083878414774E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2637,12 +2571,9 @@
       <c r="B54" s="1">
         <v>149316</v>
       </c>
-      <c r="C54" s="1">
-        <v>144593</v>
-      </c>
       <c r="D54" s="2">
         <f t="shared" si="0"/>
-        <v>3.1630903587023494E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2652,12 +2583,9 @@
       <c r="B55" s="1">
         <v>152130</v>
       </c>
-      <c r="C55" s="1">
-        <v>147243</v>
-      </c>
       <c r="D55" s="2">
         <f t="shared" si="0"/>
-        <v>3.2123841451390259E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2667,12 +2595,9 @@
       <c r="B56" s="1">
         <v>150353</v>
       </c>
-      <c r="C56" s="1">
-        <v>143261</v>
-      </c>
       <c r="D56" s="2">
         <f t="shared" si="0"/>
-        <v>4.71689956302834E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2682,12 +2607,9 @@
       <c r="B57" s="1">
         <v>150045</v>
       </c>
-      <c r="C57" s="1">
-        <v>146668</v>
-      </c>
       <c r="D57" s="2">
         <f t="shared" si="0"/>
-        <v>2.2506581358925654E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2697,12 +2619,9 @@
       <c r="B58" s="1">
         <v>148607</v>
       </c>
-      <c r="C58" s="1">
-        <v>143372</v>
-      </c>
       <c r="D58" s="2">
         <f t="shared" si="0"/>
-        <v>3.5227142732172777E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2712,12 +2631,9 @@
       <c r="B59" s="1">
         <v>149772</v>
       </c>
-      <c r="C59" s="1">
-        <v>142229</v>
-      </c>
       <c r="D59" s="2">
         <f t="shared" si="0"/>
-        <v>5.0363218759180622E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2727,12 +2643,9 @@
       <c r="B60" s="1">
         <v>155075</v>
       </c>
-      <c r="C60" s="1">
-        <v>146576</v>
-      </c>
       <c r="D60" s="2">
         <f t="shared" si="0"/>
-        <v>5.4805739158471707E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2742,12 +2655,9 @@
       <c r="B61" s="1">
         <v>154662</v>
       </c>
-      <c r="C61" s="1">
-        <v>147335</v>
-      </c>
       <c r="D61" s="2">
         <f t="shared" si="0"/>
-        <v>4.7374274223791236E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: correct some worning
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76CE233-27E4-42CB-8267-B5BB34B66813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61312016-54F9-4B5D-B7F8-A76686AD51AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:E546"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1854,15 +1854,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>22722</v>
+        <v>23237</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>6.8044788975021531E-2</v>
+        <v>4.692178335589188E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>3.4776403507067184E-2</v>
+        <v>3.0558959756265932E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>22420</v>
+        <v>21852</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>7.6378017632034279E-2</v>
+        <v>9.9777539754469805E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1888,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>21798</v>
+        <v>22034</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>7.4434206615430348E-2</v>
+        <v>6.4413400704853296E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1903,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>23354</v>
+        <v>23393</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>7.6485085408345369E-3</v>
+        <v>5.9913316903203876E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1918,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>22496</v>
+        <v>23137</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>6.2315034804718436E-2</v>
+        <v>3.5596682089116753E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>24652</v>
+        <v>24969</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>3.6692587237700754E-2</v>
+        <v>2.4305419874174516E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1963,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>22557</v>
+        <v>23043</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>3.6437419906023068E-2</v>
+        <v>1.5677061085006407E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1978,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>22540</v>
+        <v>22947</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>6.921043937892303E-2</v>
+        <v>5.2403369672943512E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1993,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>23098</v>
+        <v>22728</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>5.3787227069763632E-2</v>
+        <v>6.8944328376551553E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2008,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>42474</v>
+        <v>41982</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>6.6187992609397289E-3</v>
+        <v>1.8125687022008091E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2023,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>39563</v>
+        <v>39655</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>7.0090492419790804E-2</v>
+        <v>6.7928076154659775E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2038,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>39885</v>
+        <v>39643</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>4.9633053755242088E-2</v>
+        <v>5.5399351887152115E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2053,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>41232</v>
+        <v>42029</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>8.5562208915502327E-2</v>
+        <v>6.7886449323575071E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2068,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>39794</v>
+        <v>40035</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>5.7416267942583733E-2</v>
+        <v>5.1707802359183284E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2083,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>39636</v>
+        <v>39455</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>7.6665035991334132E-2</v>
+        <v>8.0881496494048036E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2098,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>41000</v>
+        <v>40764</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>2.4018662667523626E-2</v>
+        <v>2.9636506462900808E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2113,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>41726</v>
+        <v>42271</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>7.3167481119502442E-2</v>
+        <v>6.1061750333185248E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2128,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>41940</v>
+        <v>41819</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>3.4552611588131027E-2</v>
+        <v>3.7337998664855779E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2143,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>43110</v>
+        <v>43888</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>3.2410109081115052E-2</v>
+        <v>1.4948152803339767E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2158,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>58930</v>
+        <v>59464</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>1.4910902343619404E-2</v>
+        <v>5.9844204473270702E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>62089</v>
+        <v>62127</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-1.2886390360980011E-4</v>
+        <v>-7.409674457563506E-4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2188,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>58918</v>
+        <v>59470</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>1.4782114310558175E-2</v>
+        <v>5.551653790843116E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2203,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>60260</v>
+        <v>60226</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>3.6210916185783495E-3</v>
+        <v>4.1832702260288694E-3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2218,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>60604</v>
+        <v>60007</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>7.9717143278060596E-3</v>
+        <v>1.7744021214254144E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2233,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>58526</v>
+        <v>58747</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>7.3440865686324394E-3</v>
+        <v>3.5957190590071068E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2248,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>61853</v>
+        <v>61728</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>-5.1187883909129322E-3</v>
+        <v>-3.0875231564236731E-3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2263,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>60675</v>
+        <v>61727</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>1.3735370611183354E-2</v>
+        <v>-3.3647594278283484E-3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2278,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>59597</v>
+        <v>59348</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>-2.4220813079239064E-3</v>
+        <v>1.7661009536945149E-3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>60008</v>
+        <v>60447</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>-7.1708496623030106E-4</v>
+        <v>-8.0380221796047691E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: add best descent
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61312016-54F9-4B5D-B7F8-A76686AD51AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDCC527-C035-4A2A-A70F-ED8182797227}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="277">
   <si>
     <t>Problem</t>
   </si>
@@ -862,6 +862,9 @@
   <si>
     <t>avg</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Process finished with exit code 0</t>
   </si>
 </sst>
 </file>
@@ -1824,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C242" sqref="C242:C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1854,15 +1857,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>23237</v>
+        <v>24165</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>4.692178335589188E-2</v>
+        <v>8.8593576965669985E-3</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>3.0558959756265932E-2</v>
+        <v>-3.0421530393434051E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1876,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>21852</v>
+        <v>24351</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>9.9777539754469805E-2</v>
+        <v>-3.1721183158935485E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1891,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>22034</v>
+        <v>24284</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>6.4413400704853296E-2</v>
+        <v>-3.1123943781580399E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1906,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>23393</v>
+        <v>25361</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>5.9913316903203876E-3</v>
+        <v>-7.7632361689470547E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1921,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>23137</v>
+        <v>25331</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>3.5596682089116753E-2</v>
+        <v>-5.5854278687841277E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,11 +1936,11 @@
         <v>24613</v>
       </c>
       <c r="C7" s="1">
-        <v>24755</v>
+        <v>26710</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-5.7693089017998621E-3</v>
+        <v>-8.5198878641368381E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1951,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>24969</v>
+        <v>27541</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>2.4305419874174516E-2</v>
+        <v>-7.6198663592669302E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1966,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>23043</v>
+        <v>24045</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>1.5677061085006407E-2</v>
+        <v>-2.7125160187953867E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1981,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>22947</v>
+        <v>25264</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>5.2403369672943512E-2</v>
+        <v>-4.327717211760819E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1996,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>22728</v>
+        <v>24238</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>6.8944328376551553E-2</v>
+        <v>7.086968989390029E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2011,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>41982</v>
+        <v>44976</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>1.8125687022008091E-2</v>
+        <v>-5.1897934841078651E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2026,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>39655</v>
+        <v>42618</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>6.7928076154659775E-2</v>
+        <v>-1.7158302973322365E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2041,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>39643</v>
+        <v>43844</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>5.5399351887152115E-2</v>
+        <v>-4.4700724361418226E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2056,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>42029</v>
+        <v>44669</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>6.7886449323575071E-2</v>
+        <v>9.3368817919716116E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2071,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>40035</v>
+        <v>43383</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>5.1707802359183284E-2</v>
+        <v>-2.7594864749632859E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2086,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>39455</v>
+        <v>42151</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>8.0881496494048036E-2</v>
+        <v>1.8077200829314882E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2101,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>40764</v>
+        <v>42089</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>2.9636506462900808E-2</v>
+        <v>-1.9043538289414174E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2116,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>42271</v>
+        <v>44570</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>6.1061750333185248E-2</v>
+        <v>9.995557529986673E-3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2131,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>41819</v>
+        <v>43927</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>3.7337998664855779E-2</v>
+        <v>-1.1187587762712645E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2146,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>43888</v>
+        <v>45705</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>1.4948152803339767E-2</v>
+        <v>-2.583381963460071E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2161,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>59464</v>
+        <v>62036</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>5.9844204473270702E-3</v>
+        <v>-3.7009795727324393E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2176,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>62127</v>
+        <v>65477</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-7.409674457563506E-4</v>
+        <v>-5.4702727082360139E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2191,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>59470</v>
+        <v>61016</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>5.551653790843116E-3</v>
+        <v>-2.0300324403866091E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2206,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>60226</v>
+        <v>63149</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>4.1832702260288694E-3</v>
+        <v>-4.4147555349790833E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2221,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>60007</v>
+        <v>63075</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>1.7744021214254144E-2</v>
+        <v>-3.2476142148597995E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2236,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>58747</v>
+        <v>61201</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>3.5957190590071068E-3</v>
+        <v>-3.8026425142895913E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2251,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>61728</v>
+        <v>64734</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>-3.0875231564236731E-3</v>
+        <v>-5.1935389515421364E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2266,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>61727</v>
+        <v>63575</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>-3.3647594278283484E-3</v>
+        <v>-3.3403771131339403E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2281,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>59348</v>
+        <v>61983</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>1.7661009536945149E-3</v>
+        <v>-4.2554622979496408E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2296,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>60447</v>
+        <v>62785</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>-8.0380221796047691E-3</v>
+        <v>-4.702743266905695E-2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2319,9 +2322,12 @@
       <c r="B33" s="1">
         <v>61472</v>
       </c>
-      <c r="D33" s="2">
+      <c r="C33" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D33" s="2" t="e">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -4827,9 +4833,12 @@
       <c r="B242" s="1">
         <v>115868</v>
       </c>
+      <c r="C242" s="1">
+        <v>104870</v>
+      </c>
       <c r="D242" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>9.4918355369903687E-2</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
@@ -4839,9 +4848,12 @@
       <c r="B243" s="1">
         <v>114667</v>
       </c>
+      <c r="C243" s="1">
+        <v>103733</v>
+      </c>
       <c r="D243" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>9.5354373969843115E-2</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
@@ -4851,9 +4863,12 @@
       <c r="B244" s="1">
         <v>116661</v>
       </c>
+      <c r="C244" s="1">
+        <v>106908</v>
+      </c>
       <c r="D244" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>8.3601203487026515E-2</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
@@ -4863,9 +4878,12 @@
       <c r="B245" s="1">
         <v>115237</v>
       </c>
+      <c r="C245" s="1">
+        <v>102987</v>
+      </c>
       <c r="D245" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.10630266320712965</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
@@ -4875,9 +4893,12 @@
       <c r="B246" s="1">
         <v>116353</v>
       </c>
+      <c r="C246" s="1">
+        <v>106647</v>
+      </c>
       <c r="D246" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>8.3418562477976507E-2</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
@@ -4887,9 +4908,12 @@
       <c r="B247" s="1">
         <v>115604</v>
       </c>
+      <c r="C247" s="1">
+        <v>102998</v>
+      </c>
       <c r="D247" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.10904466973461126</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
@@ -4899,9 +4923,12 @@
       <c r="B248" s="1">
         <v>113952</v>
       </c>
+      <c r="C248" s="1">
+        <v>103276</v>
+      </c>
       <c r="D248" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>9.3688570626228582E-2</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
@@ -4911,9 +4938,12 @@
       <c r="B249" s="1">
         <v>114199</v>
       </c>
+      <c r="C249" s="1">
+        <v>103599</v>
+      </c>
       <c r="D249" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>9.2820427499365143E-2</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
@@ -4923,9 +4953,12 @@
       <c r="B250" s="1">
         <v>115247</v>
       </c>
+      <c r="C250" s="1">
+        <v>104145</v>
+      </c>
       <c r="D250" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>9.6332225567693733E-2</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
@@ -4935,9 +4968,12 @@
       <c r="B251" s="1">
         <v>116947</v>
       </c>
+      <c r="C251" s="1">
+        <v>108080</v>
+      </c>
       <c r="D251" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7.5820670902203569E-2</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
@@ -4947,9 +4983,12 @@
       <c r="B252" s="1">
         <v>217995</v>
       </c>
+      <c r="C252" s="1">
+        <v>192044</v>
+      </c>
       <c r="D252" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.11904401477098099</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
@@ -4959,9 +4998,12 @@
       <c r="B253" s="1">
         <v>214534</v>
       </c>
+      <c r="C253" s="1">
+        <v>191024</v>
+      </c>
       <c r="D253" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.10958635927172383</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
@@ -4971,9 +5013,12 @@
       <c r="B254" s="1">
         <v>215854</v>
       </c>
+      <c r="C254" s="1">
+        <v>190707</v>
+      </c>
       <c r="D254" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.1165000416948493</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
@@ -4983,9 +5028,12 @@
       <c r="B255" s="1">
         <v>217836</v>
       </c>
+      <c r="C255" s="1">
+        <v>195671</v>
+      </c>
       <c r="D255" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.10175085844396702</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
@@ -4995,9 +5043,12 @@
       <c r="B256" s="1">
         <v>215566</v>
       </c>
+      <c r="C256" s="1">
+        <v>189517</v>
+      </c>
       <c r="D256" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.12084002115361421</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.3">
@@ -5007,9 +5058,12 @@
       <c r="B257" s="1">
         <v>215762</v>
       </c>
+      <c r="C257" s="1">
+        <v>191609</v>
+      </c>
       <c r="D257" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.11194278881360017</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
@@ -5019,9 +5073,12 @@
       <c r="B258" s="1">
         <v>215772</v>
       </c>
+      <c r="C258" s="1">
+        <v>193133</v>
+      </c>
       <c r="D258" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.10492093506108299</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.3">
@@ -5031,9 +5088,12 @@
       <c r="B259" s="1">
         <v>216336</v>
       </c>
+      <c r="C259" s="1">
+        <v>194033</v>
+      </c>
       <c r="D259" s="2">
         <f t="shared" ref="D259:D271" si="4">(B259-C259)/B259</f>
-        <v>1</v>
+        <v>0.10309426077952814</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
@@ -5043,9 +5103,12 @@
       <c r="B260" s="1">
         <v>217290</v>
       </c>
+      <c r="C260" s="1">
+        <v>194908</v>
+      </c>
       <c r="D260" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.10300520042339731</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
@@ -5055,9 +5118,12 @@
       <c r="B261" s="1">
         <v>214624</v>
       </c>
+      <c r="C261" s="1">
+        <v>190405</v>
+      </c>
       <c r="D261" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.11284385716415685</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
@@ -5067,9 +5133,12 @@
       <c r="B262" s="1">
         <v>301627</v>
       </c>
+      <c r="C262" s="1">
+        <v>293027</v>
+      </c>
       <c r="D262" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2.8512036389315279E-2</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
@@ -5079,9 +5148,12 @@
       <c r="B263" s="1">
         <v>299985</v>
       </c>
+      <c r="C263" s="1">
+        <v>291678</v>
+      </c>
       <c r="D263" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2.7691384569228462E-2</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
@@ -5091,9 +5163,12 @@
       <c r="B264" s="1">
         <v>304995</v>
       </c>
+      <c r="C264" s="1">
+        <v>295336</v>
+      </c>
       <c r="D264" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.1669371629043097E-2</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
@@ -5103,9 +5178,12 @@
       <c r="B265" s="1">
         <v>301935</v>
       </c>
+      <c r="C265" s="1">
+        <v>292774</v>
+      </c>
       <c r="D265" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.0340967426764037E-2</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
@@ -5115,9 +5193,12 @@
       <c r="B266" s="1">
         <v>304404</v>
       </c>
+      <c r="C266" s="1">
+        <v>295416</v>
+      </c>
       <c r="D266" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2.9526550242440965E-2</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
@@ -5127,9 +5208,12 @@
       <c r="B267" s="1">
         <v>296894</v>
       </c>
+      <c r="C267" s="1">
+        <v>287875</v>
+      </c>
       <c r="D267" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.0377845291585548E-2</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
@@ -5139,9 +5223,12 @@
       <c r="B268" s="1">
         <v>303233</v>
       </c>
+      <c r="C268" s="1">
+        <v>293504</v>
+      </c>
       <c r="D268" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.2084238852631473E-2</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
@@ -5151,9 +5238,12 @@
       <c r="B269" s="1">
         <v>306944</v>
       </c>
+      <c r="C269" s="1">
+        <v>296365</v>
+      </c>
       <c r="D269" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.4465570266889074E-2</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
@@ -5163,9 +5253,12 @@
       <c r="B270" s="1">
         <v>303057</v>
       </c>
+      <c r="C270" s="1">
+        <v>295285</v>
+      </c>
       <c r="D270" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2.5645340645489133E-2</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
@@ -5175,9 +5268,12 @@
       <c r="B271" s="1">
         <v>300460</v>
       </c>
+      <c r="C271" s="1">
+        <v>289659</v>
+      </c>
       <c r="D271" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3.594821274046462E-2</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: delete VNS, perserve best desent
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDCC527-C035-4A2A-A70F-ED8182797227}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E34417-F61F-4757-8C45-8C84BF2C5FCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="2840" windowWidth="14070" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="best-feasible-slns" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="276">
   <si>
     <t>Problem</t>
   </si>
@@ -862,9 +862,6 @@
   <si>
     <t>avg</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Process finished with exit code 0</t>
   </si>
 </sst>
 </file>
@@ -1827,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C242" sqref="C242:C271"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1857,15 +1854,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>24165</v>
+        <v>23315</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>8.8593576965669985E-3</v>
+        <v>4.3722570854353798E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>-3.0421530393434051E-2</v>
+        <v>2.0365676258972273E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1876,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>24351</v>
+        <v>22748</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>-3.1721183158935485E-3</v>
+        <v>6.2865617533163054E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1891,11 +1888,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>24284</v>
+        <v>22173</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>-3.1123943781580399E-2</v>
+        <v>5.8511315867691392E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1906,11 +1903,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>25361</v>
+        <v>23482</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>-7.7632361689470547E-2</v>
+        <v>2.2095691340188665E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1921,11 +1918,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>25331</v>
+        <v>23160</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>-5.5854278687841277E-2</v>
+        <v>3.4637989245967241E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1936,11 +1933,11 @@
         <v>24613</v>
       </c>
       <c r="C7" s="1">
-        <v>26710</v>
+        <v>25021</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-8.5198878641368381E-2</v>
+        <v>-1.6576605858692559E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1951,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>27541</v>
+        <v>24551</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>-7.6198663592669302E-2</v>
+        <v>4.0639287249423624E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1966,11 +1963,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>24045</v>
+        <v>23443</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>-2.7125160187953867E-2</v>
+        <v>-1.4096539940196497E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1981,11 +1978,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>25264</v>
+        <v>23550</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>-4.327717211760819E-2</v>
+        <v>2.7502477700693757E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1996,11 +1993,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>24238</v>
+        <v>23005</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>7.086968989390029E-3</v>
+        <v>5.7596984965794108E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2011,11 +2008,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>44976</v>
+        <v>43035</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>-5.1897934841078651E-2</v>
+        <v>-6.501859344668709E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2026,11 +2023,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>42618</v>
+        <v>40819</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>-1.7158302973322365E-3</v>
+        <v>4.0568809495827945E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2041,11 +2038,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>43844</v>
+        <v>40509</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>-4.4700724361418226E-2</v>
+        <v>3.4764582539077389E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2056,11 +2053,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>44669</v>
+        <v>42453</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>9.3368817919716116E-3</v>
+        <v>5.8483033932135726E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2071,11 +2068,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>43383</v>
+        <v>40613</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>-2.7594864749632859E-2</v>
+        <v>3.8016959590695912E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2086,11 +2083,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>42151</v>
+        <v>39423</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>1.8077200829314882E-2</v>
+        <v>8.1626948074638342E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2101,11 +2098,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>42089</v>
+        <v>41206</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>-1.9043538289414174E-3</v>
+        <v>1.9114951557999478E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2116,11 +2113,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>44570</v>
+        <v>42286</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>9.995557529986673E-3</v>
+        <v>6.0728565082185694E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2131,11 +2128,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>43927</v>
+        <v>41867</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>-1.1187587762712645E-2</v>
+        <v>3.6233051725328605E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2146,11 +2143,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>45705</v>
+        <v>43605</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>-2.583381963460071E-2</v>
+        <v>2.1299995511065224E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2161,11 +2158,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>62036</v>
+        <v>60277</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>-3.7009795727324393E-2</v>
+        <v>-7.6058974959045166E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2176,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>65477</v>
+        <v>63154</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-5.4702727082360139E-2</v>
+        <v>-1.7283871071664438E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2191,11 +2188,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>61016</v>
+        <v>59483</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>-2.0300324403866091E-2</v>
+        <v>5.3342697568643186E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2206,11 +2203,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>63149</v>
+        <v>61255</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>-4.4147555349790833E-2</v>
+        <v>-1.2830899981811869E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2221,11 +2218,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>63075</v>
+        <v>61284</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>-3.2476142148597995E-2</v>
+        <v>-3.1592214892537363E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2236,11 +2233,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>61201</v>
+        <v>59326</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>-3.8026425142895913E-2</v>
+        <v>-6.2246645974321137E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2251,11 +2248,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>64734</v>
+        <v>62792</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>-5.1935389515421364E-2</v>
+        <v>-2.0377652832396242E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2266,11 +2263,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>63575</v>
+        <v>61562</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>-3.3403771131339403E-2</v>
+        <v>-6.8270481144343308E-4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2281,11 +2278,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>61983</v>
+        <v>60302</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>-4.2554622979496408E-2</v>
+        <v>-1.4280187711301365E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2296,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>62785</v>
+        <v>60322</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>-4.702743266905695E-2</v>
+        <v>-5.9534728591678476E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2322,12 +2319,9 @@
       <c r="B33" s="1">
         <v>61472</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D33" s="2" t="e">
+      <c r="D33" s="2">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -4833,12 +4827,9 @@
       <c r="B242" s="1">
         <v>115868</v>
       </c>
-      <c r="C242" s="1">
-        <v>104870</v>
-      </c>
       <c r="D242" s="2">
         <f t="shared" si="3"/>
-        <v>9.4918355369903687E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
@@ -4848,12 +4839,9 @@
       <c r="B243" s="1">
         <v>114667</v>
       </c>
-      <c r="C243" s="1">
-        <v>103733</v>
-      </c>
       <c r="D243" s="2">
         <f t="shared" si="3"/>
-        <v>9.5354373969843115E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
@@ -4863,12 +4851,9 @@
       <c r="B244" s="1">
         <v>116661</v>
       </c>
-      <c r="C244" s="1">
-        <v>106908</v>
-      </c>
       <c r="D244" s="2">
         <f t="shared" si="3"/>
-        <v>8.3601203487026515E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
@@ -4878,12 +4863,9 @@
       <c r="B245" s="1">
         <v>115237</v>
       </c>
-      <c r="C245" s="1">
-        <v>102987</v>
-      </c>
       <c r="D245" s="2">
         <f t="shared" si="3"/>
-        <v>0.10630266320712965</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
@@ -4893,12 +4875,9 @@
       <c r="B246" s="1">
         <v>116353</v>
       </c>
-      <c r="C246" s="1">
-        <v>106647</v>
-      </c>
       <c r="D246" s="2">
         <f t="shared" si="3"/>
-        <v>8.3418562477976507E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
@@ -4908,12 +4887,9 @@
       <c r="B247" s="1">
         <v>115604</v>
       </c>
-      <c r="C247" s="1">
-        <v>102998</v>
-      </c>
       <c r="D247" s="2">
         <f t="shared" si="3"/>
-        <v>0.10904466973461126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
@@ -4923,12 +4899,9 @@
       <c r="B248" s="1">
         <v>113952</v>
       </c>
-      <c r="C248" s="1">
-        <v>103276</v>
-      </c>
       <c r="D248" s="2">
         <f t="shared" si="3"/>
-        <v>9.3688570626228582E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.3">
@@ -4938,12 +4911,9 @@
       <c r="B249" s="1">
         <v>114199</v>
       </c>
-      <c r="C249" s="1">
-        <v>103599</v>
-      </c>
       <c r="D249" s="2">
         <f t="shared" si="3"/>
-        <v>9.2820427499365143E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.3">
@@ -4953,12 +4923,9 @@
       <c r="B250" s="1">
         <v>115247</v>
       </c>
-      <c r="C250" s="1">
-        <v>104145</v>
-      </c>
       <c r="D250" s="2">
         <f t="shared" si="3"/>
-        <v>9.6332225567693733E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
@@ -4968,12 +4935,9 @@
       <c r="B251" s="1">
         <v>116947</v>
       </c>
-      <c r="C251" s="1">
-        <v>108080</v>
-      </c>
       <c r="D251" s="2">
         <f t="shared" si="3"/>
-        <v>7.5820670902203569E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.3">
@@ -4983,12 +4947,9 @@
       <c r="B252" s="1">
         <v>217995</v>
       </c>
-      <c r="C252" s="1">
-        <v>192044</v>
-      </c>
       <c r="D252" s="2">
         <f t="shared" si="3"/>
-        <v>0.11904401477098099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
@@ -4998,12 +4959,9 @@
       <c r="B253" s="1">
         <v>214534</v>
       </c>
-      <c r="C253" s="1">
-        <v>191024</v>
-      </c>
       <c r="D253" s="2">
         <f t="shared" si="3"/>
-        <v>0.10958635927172383</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
@@ -5013,12 +4971,9 @@
       <c r="B254" s="1">
         <v>215854</v>
       </c>
-      <c r="C254" s="1">
-        <v>190707</v>
-      </c>
       <c r="D254" s="2">
         <f t="shared" si="3"/>
-        <v>0.1165000416948493</v>
+        <v>1</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
@@ -5028,12 +4983,9 @@
       <c r="B255" s="1">
         <v>217836</v>
       </c>
-      <c r="C255" s="1">
-        <v>195671</v>
-      </c>
       <c r="D255" s="2">
         <f t="shared" si="3"/>
-        <v>0.10175085844396702</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
@@ -5043,12 +4995,9 @@
       <c r="B256" s="1">
         <v>215566</v>
       </c>
-      <c r="C256" s="1">
-        <v>189517</v>
-      </c>
       <c r="D256" s="2">
         <f t="shared" si="3"/>
-        <v>0.12084002115361421</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.3">
@@ -5058,12 +5007,9 @@
       <c r="B257" s="1">
         <v>215762</v>
       </c>
-      <c r="C257" s="1">
-        <v>191609</v>
-      </c>
       <c r="D257" s="2">
         <f t="shared" si="3"/>
-        <v>0.11194278881360017</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.3">
@@ -5073,12 +5019,9 @@
       <c r="B258" s="1">
         <v>215772</v>
       </c>
-      <c r="C258" s="1">
-        <v>193133</v>
-      </c>
       <c r="D258" s="2">
         <f t="shared" si="3"/>
-        <v>0.10492093506108299</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.3">
@@ -5088,12 +5031,9 @@
       <c r="B259" s="1">
         <v>216336</v>
       </c>
-      <c r="C259" s="1">
-        <v>194033</v>
-      </c>
       <c r="D259" s="2">
         <f t="shared" ref="D259:D271" si="4">(B259-C259)/B259</f>
-        <v>0.10309426077952814</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
@@ -5103,12 +5043,9 @@
       <c r="B260" s="1">
         <v>217290</v>
       </c>
-      <c r="C260" s="1">
-        <v>194908</v>
-      </c>
       <c r="D260" s="2">
         <f t="shared" si="4"/>
-        <v>0.10300520042339731</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.3">
@@ -5118,12 +5055,9 @@
       <c r="B261" s="1">
         <v>214624</v>
       </c>
-      <c r="C261" s="1">
-        <v>190405</v>
-      </c>
       <c r="D261" s="2">
         <f t="shared" si="4"/>
-        <v>0.11284385716415685</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
@@ -5133,12 +5067,9 @@
       <c r="B262" s="1">
         <v>301627</v>
       </c>
-      <c r="C262" s="1">
-        <v>293027</v>
-      </c>
       <c r="D262" s="2">
         <f t="shared" si="4"/>
-        <v>2.8512036389315279E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
@@ -5148,12 +5079,9 @@
       <c r="B263" s="1">
         <v>299985</v>
       </c>
-      <c r="C263" s="1">
-        <v>291678</v>
-      </c>
       <c r="D263" s="2">
         <f t="shared" si="4"/>
-        <v>2.7691384569228462E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
@@ -5163,12 +5091,9 @@
       <c r="B264" s="1">
         <v>304995</v>
       </c>
-      <c r="C264" s="1">
-        <v>295336</v>
-      </c>
       <c r="D264" s="2">
         <f t="shared" si="4"/>
-        <v>3.1669371629043097E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
@@ -5178,12 +5103,9 @@
       <c r="B265" s="1">
         <v>301935</v>
       </c>
-      <c r="C265" s="1">
-        <v>292774</v>
-      </c>
       <c r="D265" s="2">
         <f t="shared" si="4"/>
-        <v>3.0340967426764037E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
@@ -5193,12 +5115,9 @@
       <c r="B266" s="1">
         <v>304404</v>
       </c>
-      <c r="C266" s="1">
-        <v>295416</v>
-      </c>
       <c r="D266" s="2">
         <f t="shared" si="4"/>
-        <v>2.9526550242440965E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
@@ -5208,12 +5127,9 @@
       <c r="B267" s="1">
         <v>296894</v>
       </c>
-      <c r="C267" s="1">
-        <v>287875</v>
-      </c>
       <c r="D267" s="2">
         <f t="shared" si="4"/>
-        <v>3.0377845291585548E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
@@ -5223,12 +5139,9 @@
       <c r="B268" s="1">
         <v>303233</v>
       </c>
-      <c r="C268" s="1">
-        <v>293504</v>
-      </c>
       <c r="D268" s="2">
         <f t="shared" si="4"/>
-        <v>3.2084238852631473E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
@@ -5238,12 +5151,9 @@
       <c r="B269" s="1">
         <v>306944</v>
       </c>
-      <c r="C269" s="1">
-        <v>296365</v>
-      </c>
       <c r="D269" s="2">
         <f t="shared" si="4"/>
-        <v>3.4465570266889074E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
@@ -5253,12 +5163,9 @@
       <c r="B270" s="1">
         <v>303057</v>
       </c>
-      <c r="C270" s="1">
-        <v>295285</v>
-      </c>
       <c r="D270" s="2">
         <f t="shared" si="4"/>
-        <v>2.5645340645489133E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
@@ -5268,12 +5175,9 @@
       <c r="B271" s="1">
         <v>300460</v>
       </c>
-      <c r="C271" s="1">
-        <v>289659</v>
-      </c>
       <c r="D271" s="2">
         <f t="shared" si="4"/>
-        <v>3.594821274046462E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: fix error caused by sorted by ratio
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E34417-F61F-4757-8C45-8C84BF2C5FCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A066414-93C3-4C07-AD08-75FCA87B8520}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="2840" windowWidth="14070" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="best-feasible-slns" sheetId="1" r:id="rId1"/>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:E546"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1854,15 +1854,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>23315</v>
+        <v>23922</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>4.3722570854353798E-2</v>
+        <v>1.8826135105204873E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>2.0365676258972273E-2</v>
+        <v>7.6385585809379481E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>22748</v>
+        <v>24008</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>6.2865617533163054E-2</v>
+        <v>1.095822690945044E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1888,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>22173</v>
+        <v>24248</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>5.8511315867691392E-2</v>
+        <v>-2.959534626979746E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1903,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>23482</v>
+        <v>23313</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>2.2095691340188665E-3</v>
+        <v>9.3906688195801811E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1918,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>23160</v>
+        <v>24709</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>3.4637989245967241E-2</v>
+        <v>-2.9927889625276146E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,11 +1933,11 @@
         <v>24613</v>
       </c>
       <c r="C7" s="1">
-        <v>25021</v>
+        <v>25496</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-1.6576605858692559E-2</v>
+        <v>-3.5875350424572378E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>24551</v>
+        <v>25489</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>4.0639287249423624E-2</v>
+        <v>3.9857762494627021E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1963,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>23443</v>
+        <v>23510</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>-1.4096539940196497E-3</v>
+        <v>-4.2716787697565147E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1978,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>23550</v>
+        <v>24385</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>2.7502477700693757E-2</v>
+        <v>-6.9788569540799473E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1993,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>23005</v>
+        <v>24368</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>5.7596984965794108E-2</v>
+        <v>1.7615009626807587E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2008,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>43035</v>
+        <v>41955</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>-6.501859344668709E-3</v>
+        <v>1.8757162569871599E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2023,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>40819</v>
+        <v>41201</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>4.0568809495827945E-2</v>
+        <v>3.1590081090609942E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2038,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>40509</v>
+        <v>41729</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>3.4764582539077389E-2</v>
+        <v>5.694815097216927E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2053,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>42453</v>
+        <v>43021</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>5.8483033932135726E-2</v>
+        <v>4.588600576624529E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2068,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>40613</v>
+        <v>40829</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>3.8016959590695912E-2</v>
+        <v>3.2900658486901324E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2083,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>39423</v>
+        <v>41028</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>8.1626948074638342E-2</v>
+        <v>4.4237892235655878E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2098,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>41206</v>
+        <v>40077</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>1.9114951557999478E-2</v>
+        <v>4.5990144968935227E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2113,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>42286</v>
+        <v>43892</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>6.0728565082185694E-2</v>
+        <v>2.5055530875166591E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2128,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>41867</v>
+        <v>43449</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>3.6233051725328605E-2</v>
+        <v>-1.8415782325452914E-4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2143,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>43605</v>
+        <v>44177</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>2.1299995511065224E-2</v>
+        <v>8.4616420523409789E-3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2158,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>60277</v>
+        <v>60079</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>-7.6058974959045166E-3</v>
+        <v>-4.2960783658185951E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>63154</v>
+        <v>62160</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-1.7283871071664438E-2</v>
+        <v>-1.272531048146776E-3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2188,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>59483</v>
+        <v>59439</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>5.3342697568643186E-3</v>
+        <v>6.0700311026387075E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2203,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>61255</v>
+        <v>60077</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>-1.2830899981811869E-2</v>
+        <v>6.6469352998561482E-3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2218,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>61284</v>
+        <v>60412</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>-3.1592214892537363E-3</v>
+        <v>1.1114566793799414E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2233,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>59326</v>
+        <v>59430</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>-6.2246645974321137E-3</v>
+        <v>-7.9886022490205065E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2248,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>62792</v>
+        <v>61439</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>-2.0377652832396242E-2</v>
+        <v>1.6087620657154929E-3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2263,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>61562</v>
+        <v>61071</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>-6.8270481144343308E-4</v>
+        <v>7.2984395318595576E-3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2278,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>60302</v>
+        <v>58841</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>-1.4280187711301365E-2</v>
+        <v>1.0293845558676601E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>60322</v>
+        <v>59784</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>-5.9534728591678476E-3</v>
+        <v>3.0184274159926624E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: fixed the bug caused by sorted by ration
after sorted by ration, the order has been changed, and the feasibility should be calculated in a
new way
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC72125-E5CA-4010-BD3A-A5006DA1FEBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2052B36E-55D3-42E9-AC08-DA81D3930EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:E546"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1854,15 +1854,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>22408</v>
+        <v>23922</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>8.0923670070956896E-2</v>
+        <v>1.8826135105204873E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>1.5978611400744545E-2</v>
+        <v>6.1078138994915317E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>22799</v>
+        <v>24717</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>6.0764604103155637E-2</v>
+        <v>-1.8249979401829118E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1888,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>22146</v>
+        <v>24623</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>5.9657764001528599E-2</v>
+        <v>-4.5518237017536413E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1903,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>24225</v>
+        <v>23313</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>-2.9361774453981474E-2</v>
+        <v>9.3906688195801811E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1918,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>22788</v>
+        <v>24709</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>5.0143803926472427E-2</v>
+        <v>-2.9927889625276146E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,11 +1933,11 @@
         <v>24613</v>
       </c>
       <c r="C7" s="1">
-        <v>25419</v>
+        <v>25496</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-3.274692235810344E-2</v>
+        <v>-3.5875350424572378E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>25399</v>
+        <v>25470</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>7.5026376460474381E-3</v>
+        <v>4.7282247665194795E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1963,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>23400</v>
+        <v>23510</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>4.2716787697565144E-4</v>
+        <v>-4.2716787697565147E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1978,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>24000</v>
+        <v>24385</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>8.9197224975222991E-3</v>
+        <v>-6.9788569540799473E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1993,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>23252</v>
+        <v>24368</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>4.7478595715046493E-2</v>
+        <v>1.7615009626807587E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2008,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>44255</v>
+        <v>41955</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>-3.5035198914797575E-2</v>
+        <v>1.8757162569871599E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2023,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>42484</v>
+        <v>41201</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>1.4337760018803621E-3</v>
+        <v>3.1590081090609942E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2038,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>41209</v>
+        <v>41729</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>1.8085207777354173E-2</v>
+        <v>5.694815097216927E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2053,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>41720</v>
+        <v>43021</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>7.4739410068751386E-2</v>
+        <v>4.588600576624529E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2068,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>40307</v>
+        <v>40829</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>4.5265052821071579E-2</v>
+        <v>3.2900658486901324E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2083,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>40425</v>
+        <v>41028</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>5.8284995457404433E-2</v>
+        <v>4.4237892235655878E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2098,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>40976</v>
+        <v>40077</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>2.4589968816206051E-2</v>
+        <v>4.5990144968935227E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2113,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>43089</v>
+        <v>43892</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>4.2892047978676143E-2</v>
+        <v>2.5055530875166591E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2128,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>42157</v>
+        <v>43449</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>2.9557330632351924E-2</v>
+        <v>-1.8415782325452914E-4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2143,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>44326</v>
+        <v>44177</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>5.117385644386587E-3</v>
+        <v>8.4616420523409789E-3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2158,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>59249</v>
+        <v>60079</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>9.5784159673698646E-3</v>
+        <v>-4.2960783658185951E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>63154</v>
+        <v>62160</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-1.7283871071664438E-2</v>
+        <v>-1.272531048146776E-3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2188,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>59610</v>
+        <v>59439</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>3.2105949633791514E-3</v>
+        <v>6.0700311026387075E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2203,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>60956</v>
+        <v>60077</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>-7.8870351692322954E-3</v>
+        <v>6.6469352998561482E-3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2218,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>60785</v>
+        <v>60468</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>5.0089211176769085E-3</v>
+        <v>1.0197901491218018E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2233,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>59085</v>
+        <v>59430</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>-2.1370783086551671E-3</v>
+        <v>-7.9886022490205065E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2248,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>62424</v>
+        <v>61439</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>-1.4397607982059865E-2</v>
+        <v>1.6087620657154929E-3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2263,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>61710</v>
+        <v>61071</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>-3.0884265279583875E-3</v>
+        <v>7.2984395318595576E-3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2278,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>59994</v>
+        <v>58841</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>-9.0996249137974532E-3</v>
+        <v>1.0293845558676601E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>60156</v>
+        <v>59821</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>-3.1851913616276163E-3</v>
+        <v>2.4014008171433336E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: first try of penalty
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A066414-93C3-4C07-AD08-75FCA87B8520}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EAFBE3-58AF-4E02-8EA7-761861FBB102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:E546"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>7.6385585809379481E-3</v>
+        <v>6.4034814524298435E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>24008</v>
+        <v>24717</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>1.095822690945044E-2</v>
+        <v>-1.8249979401829118E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1888,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>24248</v>
+        <v>24430</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>-2.959534626979746E-2</v>
+        <v>-3.7323255912700096E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>25489</v>
+        <v>25470</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>3.9857762494627021E-3</v>
+        <v>4.7282247665194795E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>62160</v>
+        <v>62175</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-1.272531048146776E-3</v>
+        <v>-1.5141508674151511E-3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>59784</v>
+        <v>59821</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>3.0184274159926624E-3</v>
+        <v>2.4014008171433336E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: add vns neighbor
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2052B36E-55D3-42E9-AC08-DA81D3930EE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF5EDDF-8D04-4C88-B73E-5AE60E3D0023}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1824,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="E226" sqref="E226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1854,15 +1854,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>23922</v>
+        <v>24450</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>1.8826135105204873E-2</v>
+        <v>-2.8300725975144579E-3</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>6.1078138994915317E-3</v>
+        <v>-9.5859493907530392E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>24717</v>
+        <v>25046</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>-1.8249979401829118E-2</v>
+        <v>-3.1803575842465188E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1903,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>23313</v>
+        <v>23729</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>9.3906688195801811E-3</v>
+        <v>-8.2858842525707493E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1918,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>24709</v>
+        <v>24922</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>-2.9927889625276146E-2</v>
+        <v>-3.8806218998791213E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,11 +1933,11 @@
         <v>24613</v>
       </c>
       <c r="C7" s="1">
-        <v>25496</v>
+        <v>25828</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-3.5875350424572378E-2</v>
+        <v>-4.9364157152724172E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>25470</v>
+        <v>25558</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>4.7282247665194795E-3</v>
+        <v>1.2895158454144036E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1963,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>23510</v>
+        <v>24159</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>-4.2716787697565147E-3</v>
+        <v>-3.1994873985476291E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1978,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>24385</v>
+        <v>25029</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>-6.9788569540799473E-3</v>
+        <v>-3.3572844400396429E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1993,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>24368</v>
+        <v>24665</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>1.7615009626807587E-3</v>
+        <v>-1.0405145221416574E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2008,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>41955</v>
+        <v>42632</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>1.8757162569871599E-2</v>
+        <v>2.9234979067754986E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2023,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>41201</v>
+        <v>42039</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>3.1590081090609942E-2</v>
+        <v>1.1893289458220708E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2038,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>41729</v>
+        <v>42340</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>5.694815097216927E-3</v>
+        <v>-8.8638963019443389E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2053,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>43021</v>
+        <v>45134</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>4.588600576624529E-2</v>
+        <v>-9.7582612552672438E-4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2068,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>40829</v>
+        <v>42140</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>3.2900658486901324E-2</v>
+        <v>1.8475531763702687E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2083,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>41028</v>
+        <v>43451</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>4.4237892235655878E-2</v>
+        <v>-1.2206769632166235E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2098,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>40077</v>
+        <v>41807</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>4.5990144968935227E-2</v>
+        <v>4.8084934180770787E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2113,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>43892</v>
+        <v>45354</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>2.5055530875166591E-2</v>
+        <v>-7.4189249222567748E-3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2128,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>43449</v>
+        <v>44610</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>-1.8415782325452914E-4</v>
+        <v>-2.6910061923068069E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2143,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>44177</v>
+        <v>43753</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>8.4616420523409789E-3</v>
+        <v>1.7978183776989721E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2158,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>60079</v>
+        <v>60278</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>-4.2960783658185951E-3</v>
+        <v>-7.6226137541372738E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>62160</v>
+        <v>62607</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-1.272531048146776E-3</v>
+        <v>-8.4728016623443567E-3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2188,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>59439</v>
+        <v>59760</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>6.0700311026387075E-3</v>
+        <v>7.0231764823918937E-4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2203,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>60077</v>
+        <v>60390</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>6.6469352998561482E-3</v>
+        <v>1.4715851783263611E-3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2218,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>60468</v>
+        <v>61324</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>1.0197901491218018E-2</v>
+        <v>-3.8139824196690183E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2233,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>59430</v>
+        <v>59200</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>-7.9886022490205065E-3</v>
+        <v>-4.0875862887769466E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2248,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>61439</v>
+        <v>61550</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>1.6087620657154929E-3</v>
+        <v>-1.9500146251096883E-4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2263,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>61071</v>
+        <v>61342</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>7.2984395318595576E-3</v>
+        <v>2.893368010403121E-3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2278,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>58841</v>
+        <v>59251</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>1.0293845558676601E-2</v>
+        <v>3.3976418347265907E-3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>59821</v>
+        <v>60183</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>2.4014008171433336E-3</v>
+        <v>-3.6354540148419911E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -4467,13 +4467,16 @@
       <c r="B212" s="1">
         <v>56693</v>
       </c>
+      <c r="C212" s="1">
+        <v>52928</v>
+      </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6.6410315206462872E-2</v>
       </c>
       <c r="E212" s="2">
         <f>AVERAGE(D212:D241)</f>
-        <v>1</v>
+        <v>5.4441791582874183E-2</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
@@ -4483,9 +4486,12 @@
       <c r="B213" s="1">
         <v>58318</v>
       </c>
+      <c r="C213" s="1">
+        <v>55108</v>
+      </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5.5043039884769711E-2</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
@@ -4495,9 +4501,12 @@
       <c r="B214" s="1">
         <v>56553</v>
       </c>
+      <c r="C214" s="1">
+        <v>52365</v>
+      </c>
       <c r="D214" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7.4054426820858305E-2</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
@@ -4507,9 +4516,12 @@
       <c r="B215" s="1">
         <v>56863</v>
       </c>
+      <c r="C215" s="1">
+        <v>53315</v>
+      </c>
       <c r="D215" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6.2395582364630782E-2</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
@@ -4519,9 +4531,12 @@
       <c r="B216" s="1">
         <v>56629</v>
       </c>
+      <c r="C216" s="1">
+        <v>52510</v>
+      </c>
       <c r="D216" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7.2736583729184692E-2</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
@@ -4531,9 +4546,12 @@
       <c r="B217" s="1">
         <v>57119</v>
       </c>
+      <c r="C217" s="1">
+        <v>53291</v>
+      </c>
       <c r="D217" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6.701798000665278E-2</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
@@ -4543,9 +4561,12 @@
       <c r="B218" s="1">
         <v>56292</v>
       </c>
+      <c r="C218" s="1">
+        <v>52596</v>
+      </c>
       <c r="D218" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6.5657642293753996E-2</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
@@ -4555,9 +4576,12 @@
       <c r="B219" s="1">
         <v>56403</v>
       </c>
+      <c r="C219" s="1">
+        <v>52303</v>
+      </c>
       <c r="D219" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7.2691168909455164E-2</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
@@ -4567,9 +4591,12 @@
       <c r="B220" s="1">
         <v>57442</v>
       </c>
+      <c r="C220" s="1">
+        <v>53839</v>
+      </c>
       <c r="D220" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6.2724139131645831E-2</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
@@ -4579,9 +4606,12 @@
       <c r="B221" s="1">
         <v>56447</v>
       </c>
+      <c r="C221" s="1">
+        <v>52129</v>
+      </c>
       <c r="D221" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7.6496536574131482E-2</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
@@ -4591,9 +4621,12 @@
       <c r="B222" s="1">
         <v>107689</v>
       </c>
+      <c r="C222" s="1">
+        <v>102563</v>
+      </c>
       <c r="D222" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4.7600033429598197E-2</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
@@ -4603,9 +4636,12 @@
       <c r="B223" s="1">
         <v>108338</v>
       </c>
+      <c r="C223" s="1">
+        <v>101032</v>
+      </c>
       <c r="D223" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6.7437095017445409E-2</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
@@ -4615,9 +4651,12 @@
       <c r="B224" s="1">
         <v>106385</v>
       </c>
+      <c r="C224" s="1">
+        <v>100470</v>
+      </c>
       <c r="D224" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5.559994360107158E-2</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
@@ -4627,9 +4666,12 @@
       <c r="B225" s="1">
         <v>106796</v>
       </c>
+      <c r="C225" s="1">
+        <v>98965</v>
+      </c>
       <c r="D225" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7.332671635641784E-2</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
@@ -4639,9 +4681,12 @@
       <c r="B226" s="1">
         <v>107396</v>
       </c>
+      <c r="C226" s="1">
+        <v>100133</v>
+      </c>
       <c r="D226" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>6.7628217065812513E-2</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
@@ -4651,9 +4696,12 @@
       <c r="B227" s="1">
         <v>107246</v>
       </c>
+      <c r="C227" s="1">
+        <v>97511</v>
+      </c>
       <c r="D227" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>9.0772616228111072E-2</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
@@ -4663,9 +4711,12 @@
       <c r="B228" s="1">
         <v>106308</v>
       </c>
+      <c r="C228" s="1">
+        <v>97432</v>
+      </c>
       <c r="D228" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>8.3493246039808858E-2</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
@@ -4675,9 +4726,12 @@
       <c r="B229" s="1">
         <v>103993</v>
       </c>
+      <c r="C229" s="1">
+        <v>96133</v>
+      </c>
       <c r="D229" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7.5582010327618201E-2</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
@@ -4687,9 +4741,12 @@
       <c r="B230" s="1">
         <v>106835</v>
       </c>
+      <c r="C230" s="1">
+        <v>98233</v>
+      </c>
       <c r="D230" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>8.0516684607104413E-2</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
@@ -4699,9 +4756,12 @@
       <c r="B231" s="1">
         <v>105751</v>
       </c>
+      <c r="C231" s="1">
+        <v>99862</v>
+      </c>
       <c r="D231" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5.5687416667454678E-2</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
@@ -4711,9 +4771,12 @@
       <c r="B232" s="1">
         <v>150083</v>
       </c>
+      <c r="C232" s="1">
+        <v>146225</v>
+      </c>
       <c r="D232" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.5705776137204081E-2</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
@@ -4723,9 +4786,12 @@
       <c r="B233" s="1">
         <v>149907</v>
       </c>
+      <c r="C233" s="1">
+        <v>146249</v>
+      </c>
       <c r="D233" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.4401795780050299E-2</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
@@ -4735,9 +4801,12 @@
       <c r="B234" s="1">
         <v>152993</v>
       </c>
+      <c r="C234" s="1">
+        <v>149089</v>
+      </c>
       <c r="D234" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.5517507336936984E-2</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
@@ -4747,9 +4816,12 @@
       <c r="B235" s="1">
         <v>153169</v>
       </c>
+      <c r="C235" s="1">
+        <v>149058</v>
+      </c>
       <c r="D235" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.6839634651920428E-2</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
@@ -4759,9 +4831,12 @@
       <c r="B236" s="1">
         <v>150287</v>
       </c>
+      <c r="C236" s="1">
+        <v>147160</v>
+      </c>
       <c r="D236" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.0806856215108426E-2</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
@@ -4771,9 +4846,12 @@
       <c r="B237" s="1">
         <v>148544</v>
       </c>
+      <c r="C237" s="1">
+        <v>144512</v>
+      </c>
       <c r="D237" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.7143472641102971E-2</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
@@ -4783,9 +4861,12 @@
       <c r="B238" s="1">
         <v>147471</v>
       </c>
+      <c r="C238" s="1">
+        <v>142847</v>
+      </c>
       <c r="D238" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.1355317316624963E-2</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
@@ -4795,9 +4876,12 @@
       <c r="B239" s="1">
         <v>152841</v>
       </c>
+      <c r="C239" s="1">
+        <v>149149</v>
+      </c>
       <c r="D239" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.415582206345156E-2</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
@@ -4807,9 +4891,12 @@
       <c r="B240" s="1">
         <v>149568</v>
       </c>
+      <c r="C240" s="1">
+        <v>145140</v>
+      </c>
       <c r="D240" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.9605263157894735E-2</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
@@ -4819,9 +4906,12 @@
       <c r="B241" s="1">
         <v>149572</v>
       </c>
+      <c r="C241" s="1">
+        <v>145855</v>
+      </c>
       <c r="D241" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.4850907923942983E-2</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refactor: remove vns and best descent
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EAFBE3-58AF-4E02-8EA7-761861FBB102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BBDAF7-B3A2-4686-A8F3-CD0DE3654553}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1854,15 +1854,15 @@
         <v>24381</v>
       </c>
       <c r="C2" s="1">
-        <v>23922</v>
+        <v>23067</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>1.8826135105204873E-2</v>
+        <v>5.3894425987449243E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>6.4034814524298435E-3</v>
+        <v>3.0142855661636984E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1873,11 @@
         <v>24274</v>
       </c>
       <c r="C3" s="1">
-        <v>24717</v>
+        <v>23295</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>-1.8249979401829118E-2</v>
+        <v>4.0331218587789402E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1888,11 @@
         <v>23551</v>
       </c>
       <c r="C4" s="1">
-        <v>24430</v>
+        <v>22887</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>-3.7323255912700096E-2</v>
+        <v>2.8194131883996432E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1903,11 @@
         <v>23534</v>
       </c>
       <c r="C5" s="1">
-        <v>23313</v>
+        <v>22003</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>9.3906688195801811E-3</v>
+        <v>6.5054814311209311E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1918,11 @@
         <v>23991</v>
       </c>
       <c r="C6" s="1">
-        <v>24709</v>
+        <v>23072</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>-2.9927889625276146E-2</v>
+        <v>3.8306031428452333E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,11 +1933,11 @@
         <v>24613</v>
       </c>
       <c r="C7" s="1">
-        <v>25496</v>
+        <v>23976</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-3.5875350424572378E-2</v>
+        <v>2.5880632186243042E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1948,11 @@
         <v>25591</v>
       </c>
       <c r="C8" s="1">
-        <v>25470</v>
+        <v>24326</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>4.7282247665194795E-3</v>
+        <v>4.9431440740885464E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1963,11 @@
         <v>23410</v>
       </c>
       <c r="C9" s="1">
-        <v>23510</v>
+        <v>22942</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>-4.2716787697565147E-3</v>
+        <v>1.9991456642460485E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1978,11 @@
         <v>24216</v>
       </c>
       <c r="C10" s="1">
-        <v>24385</v>
+        <v>23192</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>-6.9788569540799473E-3</v>
+        <v>4.2286091840105712E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1993,11 @@
         <v>24411</v>
       </c>
       <c r="C11" s="1">
-        <v>24368</v>
+        <v>23956</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>1.7615009626807587E-3</v>
+        <v>1.8639138093482447E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2008,11 @@
         <v>42757</v>
       </c>
       <c r="C12" s="1">
-        <v>41955</v>
+        <v>41124</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>1.8757162569871599E-2</v>
+        <v>3.8192576654115115E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2023,11 @@
         <v>42545</v>
       </c>
       <c r="C13" s="1">
-        <v>41201</v>
+        <v>40847</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>3.1590081090609942E-2</v>
+        <v>3.9910682806440237E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2038,11 @@
         <v>41968</v>
       </c>
       <c r="C14" s="1">
-        <v>41729</v>
+        <v>40503</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>5.694815097216927E-3</v>
+        <v>3.4907548608463589E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2053,11 @@
         <v>45090</v>
       </c>
       <c r="C15" s="1">
-        <v>43021</v>
+        <v>43163</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>4.588600576624529E-2</v>
+        <v>4.2736748724772677E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2068,11 @@
         <v>42218</v>
       </c>
       <c r="C16" s="1">
-        <v>40829</v>
+        <v>40707</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>3.2900658486901324E-2</v>
+        <v>3.5790421147377897E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2083,11 @@
         <v>42927</v>
       </c>
       <c r="C17" s="1">
-        <v>41028</v>
+        <v>41061</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>4.4237892235655878E-2</v>
+        <v>4.3469145293172126E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2098,11 @@
         <v>42009</v>
       </c>
       <c r="C18" s="1">
-        <v>40077</v>
+        <v>40528</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>4.5990144968935227E-2</v>
+        <v>3.5254350258277986E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2113,11 @@
         <v>45020</v>
       </c>
       <c r="C19" s="1">
-        <v>43892</v>
+        <v>42859</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>2.5055530875166591E-2</v>
+        <v>4.8000888494002664E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2128,11 @@
         <v>43441</v>
       </c>
       <c r="C20" s="1">
-        <v>43449</v>
+        <v>41539</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>-1.8415782325452914E-4</v>
+        <v>4.3783522478764304E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2143,11 @@
         <v>44554</v>
       </c>
       <c r="C21" s="1">
-        <v>44177</v>
+        <v>41974</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>8.4616420523409789E-3</v>
+        <v>5.790725860753243E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2158,11 @@
         <v>59822</v>
       </c>
       <c r="C22" s="1">
-        <v>60079</v>
+        <v>59412</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>-4.2960783658185951E-3</v>
+        <v>6.8536658754304435E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2173,11 @@
         <v>62081</v>
       </c>
       <c r="C23" s="1">
-        <v>62175</v>
+        <v>62008</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-1.5141508674151511E-3</v>
+        <v>1.175883120439426E-3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2188,11 @@
         <v>59802</v>
       </c>
       <c r="C24" s="1">
-        <v>59439</v>
+        <v>59299</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>6.0700311026387075E-3</v>
+        <v>8.411089930102672E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2203,11 @@
         <v>60479</v>
       </c>
       <c r="C25" s="1">
-        <v>60077</v>
+        <v>59815</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>6.6469352998561482E-3</v>
+        <v>1.0979017510210156E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2218,11 @@
         <v>61091</v>
       </c>
       <c r="C26" s="1">
-        <v>60412</v>
+        <v>60043</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>1.1114566793799414E-2</v>
+        <v>1.7154736376880392E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2233,11 @@
         <v>58959</v>
       </c>
       <c r="C27" s="1">
-        <v>59430</v>
+        <v>58338</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>-7.9886022490205065E-3</v>
+        <v>1.053274309265761E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2248,11 @@
         <v>61538</v>
       </c>
       <c r="C28" s="1">
-        <v>61439</v>
+        <v>60718</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>1.6087620657154929E-3</v>
+        <v>1.3325099938249537E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2263,11 @@
         <v>61520</v>
       </c>
       <c r="C29" s="1">
-        <v>61071</v>
+        <v>60478</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>7.2984395318595576E-3</v>
+        <v>1.6937581274382316E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2278,11 @@
         <v>59453</v>
       </c>
       <c r="C30" s="1">
-        <v>58841</v>
+        <v>58802</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>1.0293845558676601E-2</v>
+        <v>1.0949825912905994E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2293,11 @@
         <v>59965</v>
       </c>
       <c r="C31" s="1">
-        <v>59821</v>
+        <v>59605</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>2.4014008171433336E-3</v>
+        <v>6.003502042858334E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: add new VNS
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BBDAF7-B3A2-4686-A8F3-CD0DE3654553}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2372264E-337E-436A-ACEF-ABE529250DBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1824,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1851,18 +1851,18 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>24381</v>
+        <v>24038</v>
       </c>
       <c r="C2" s="1">
-        <v>23067</v>
+        <v>23326</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>5.3894425987449243E-2</v>
+        <v>2.961976869955903E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>3.0142855661636984E-2</v>
+        <v>7.6996391482580442E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1870,14 +1870,14 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>24274</v>
+        <v>24620</v>
       </c>
       <c r="C3" s="1">
-        <v>23295</v>
+        <v>24114</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>4.0331218587789402E-2</v>
+        <v>2.0552396425670187E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1885,14 +1885,14 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>23551</v>
+        <v>24347</v>
       </c>
       <c r="C4" s="1">
-        <v>22887</v>
+        <v>23959</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>2.8194131883996432E-2</v>
+        <v>1.5936254980079681E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1900,14 +1900,14 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>23534</v>
+        <v>22913</v>
       </c>
       <c r="C5" s="1">
-        <v>22003</v>
+        <v>22709</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>6.5054814311209311E-2</v>
+        <v>8.9032427006502865E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1915,14 +1915,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>23991</v>
+        <v>24664</v>
       </c>
       <c r="C6" s="1">
-        <v>23072</v>
+        <v>24219</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>3.8306031428452333E-2</v>
+        <v>1.8042491080116768E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1930,14 +1930,14 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>24613</v>
+        <v>24906</v>
       </c>
       <c r="C7" s="1">
-        <v>23976</v>
+        <v>25258</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>2.5880632186243042E-2</v>
+        <v>-1.413314060868867E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1945,14 +1945,14 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>25591</v>
+        <v>25313</v>
       </c>
       <c r="C8" s="1">
-        <v>24326</v>
+        <v>25071</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>4.9431440740885464E-2</v>
+        <v>9.5603049816299929E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1960,14 +1960,14 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>23410</v>
+        <v>23366</v>
       </c>
       <c r="C9" s="1">
-        <v>22942</v>
+        <v>23337</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>1.9991456642460485E-2</v>
+        <v>1.2411195754515108E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1975,14 +1975,14 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>24216</v>
+        <v>24756</v>
       </c>
       <c r="C10" s="1">
-        <v>23192</v>
+        <v>24365</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>4.2286091840105712E-2</v>
+        <v>1.5794150912910001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1990,14 +1990,14 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>24411</v>
+        <v>24096</v>
       </c>
       <c r="C11" s="1">
-        <v>23956</v>
+        <v>24220</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>1.8639138093482447E-2</v>
+        <v>-5.1460823373173968E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2005,14 +2005,14 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>42757</v>
+        <v>42505</v>
       </c>
       <c r="C12" s="1">
-        <v>41124</v>
+        <v>41351</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>3.8192576654115115E-2</v>
+        <v>2.7149747088577814E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2020,14 +2020,14 @@
         <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>42545</v>
+        <v>41934</v>
       </c>
       <c r="C13" s="1">
-        <v>40847</v>
+        <v>40983</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>3.9910682806440237E-2</v>
+        <v>2.267849477750751E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2035,14 +2035,14 @@
         <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>41968</v>
+        <v>41737</v>
       </c>
       <c r="C14" s="1">
-        <v>40503</v>
+        <v>41417</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>3.4907548608463589E-2</v>
+        <v>7.6670580060857274E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2050,14 +2050,14 @@
         <v>15</v>
       </c>
       <c r="B15" s="1">
-        <v>45090</v>
+        <v>44801</v>
       </c>
       <c r="C15" s="1">
-        <v>43163</v>
+        <v>43992</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>4.2736748724772677E-2</v>
+        <v>1.8057632642128525E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2065,14 +2065,14 @@
         <v>16</v>
       </c>
       <c r="B16" s="1">
-        <v>42218</v>
+        <v>42001</v>
       </c>
       <c r="C16" s="1">
-        <v>40707</v>
+        <v>40717</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>3.5790421147377897E-2</v>
+        <v>3.0570700697602437E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2080,14 +2080,14 @@
         <v>17</v>
       </c>
       <c r="B17" s="1">
-        <v>42927</v>
+        <v>42946</v>
       </c>
       <c r="C17" s="1">
-        <v>41061</v>
+        <v>42666</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>4.3469145293172126E-2</v>
+        <v>6.5198155823592415E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2095,14 +2095,14 @@
         <v>18</v>
       </c>
       <c r="B18" s="1">
-        <v>42009</v>
+        <v>41607</v>
       </c>
       <c r="C18" s="1">
-        <v>40528</v>
+        <v>40661</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>3.5254350258277986E-2</v>
+        <v>2.2736558752133054E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,14 +2110,14 @@
         <v>19</v>
       </c>
       <c r="B19" s="1">
-        <v>45020</v>
+        <v>44441</v>
       </c>
       <c r="C19" s="1">
-        <v>42859</v>
+        <v>44243</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>4.8000888494002664E-2</v>
+        <v>4.4553452892599175E-3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2125,14 +2125,14 @@
         <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>43441</v>
+        <v>43372</v>
       </c>
       <c r="C20" s="1">
-        <v>41539</v>
+        <v>43664</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>4.3783522478764304E-2</v>
+        <v>-6.7324541178640594E-3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2140,14 +2140,14 @@
         <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>44554</v>
+        <v>44275</v>
       </c>
       <c r="C21" s="1">
-        <v>41974</v>
+        <v>43837</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>5.790725860753243E-2</v>
+        <v>9.892715979672501E-3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2155,14 +2155,14 @@
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>59822</v>
+        <v>60105</v>
       </c>
       <c r="C22" s="1">
-        <v>59412</v>
+        <v>59910</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>6.8536658754304435E-3</v>
+        <v>3.2443224357374596E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2170,14 +2170,14 @@
         <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>62081</v>
+        <v>62231</v>
       </c>
       <c r="C23" s="1">
-        <v>62008</v>
+        <v>62514</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>1.175883120439426E-3</v>
+        <v>-4.5475727531294691E-3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2185,14 +2185,14 @@
         <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>59802</v>
+        <v>59807</v>
       </c>
       <c r="C24" s="1">
-        <v>59299</v>
+        <v>59708</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>8.411089930102672E-3</v>
+        <v>1.6553246275519589E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2200,14 +2200,14 @@
         <v>25</v>
       </c>
       <c r="B25" s="1">
-        <v>60479</v>
+        <v>60379</v>
       </c>
       <c r="C25" s="1">
-        <v>59815</v>
+        <v>60319</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>1.0979017510210156E-2</v>
+        <v>9.9372298315639554E-4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2215,14 +2215,14 @@
         <v>26</v>
       </c>
       <c r="B26" s="1">
-        <v>61091</v>
+        <v>60700</v>
       </c>
       <c r="C26" s="1">
-        <v>60043</v>
+        <v>61043</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>1.7154736376880392E-2</v>
+        <v>-5.6507413509060958E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2230,14 +2230,14 @@
         <v>27</v>
       </c>
       <c r="B27" s="1">
-        <v>58959</v>
+        <v>59328</v>
       </c>
       <c r="C27" s="1">
-        <v>58338</v>
+        <v>58889</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>1.053274309265761E-2</v>
+        <v>7.3995415318230855E-3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2245,14 +2245,14 @@
         <v>28</v>
       </c>
       <c r="B28" s="1">
-        <v>61538</v>
+        <v>60852</v>
       </c>
       <c r="C28" s="1">
-        <v>60718</v>
+        <v>60911</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>1.3325099938249537E-2</v>
+        <v>-9.6956550318806286E-4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2260,14 +2260,14 @@
         <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>61520</v>
+        <v>60409</v>
       </c>
       <c r="C29" s="1">
-        <v>60478</v>
+        <v>61017</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>1.6937581274382316E-2</v>
+        <v>-1.0064725454816336E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2275,14 +2275,14 @@
         <v>30</v>
       </c>
       <c r="B30" s="1">
-        <v>59453</v>
+        <v>59073</v>
       </c>
       <c r="C30" s="1">
-        <v>58802</v>
+        <v>59146</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>1.0949825912905994E-2</v>
+        <v>-1.2357591454640869E-3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2290,14 +2290,14 @@
         <v>31</v>
       </c>
       <c r="B31" s="1">
-        <v>59965</v>
+        <v>59972</v>
       </c>
       <c r="C31" s="1">
-        <v>59605</v>
+        <v>60164</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>6.003502042858334E-3</v>
+        <v>-3.2014940305475888E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -4467,9 +4467,12 @@
       <c r="B212" s="1">
         <v>56693</v>
       </c>
+      <c r="C212" s="1">
+        <v>54442</v>
+      </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.970507822835271E-2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4479,9 +4482,12 @@
       <c r="B213" s="1">
         <v>58318</v>
       </c>
+      <c r="C213" s="1">
+        <v>55460</v>
+      </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4.9007167598340132E-2</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
@@ -4491,9 +4497,12 @@
       <c r="B214" s="1">
         <v>56553</v>
       </c>
+      <c r="C214" s="1">
+        <v>53504</v>
+      </c>
       <c r="D214" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5.3914027549378456E-2</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: change the way to find the global best
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2372264E-337E-436A-ACEF-ABE529250DBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B8E3ED-BEF0-405B-BB78-4998CE22E101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="277">
   <si>
     <t>Problem</t>
   </si>
@@ -862,6 +862,9 @@
   <si>
     <t>avg</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Starting the run!</t>
   </si>
 </sst>
 </file>
@@ -1824,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1839,6 +1842,9 @@
       <c r="B1" s="1" t="s">
         <v>273</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="D1" s="2" t="s">
         <v>274</v>
       </c>
@@ -1854,15 +1860,15 @@
         <v>24038</v>
       </c>
       <c r="C2" s="1">
-        <v>23326</v>
+        <v>24373</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>2.961976869955903E-2</v>
+        <v>-1.3936267576337466E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>7.6996391482580442E-3</v>
+        <v>-9.6011628899455824E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1873,11 +1879,11 @@
         <v>24620</v>
       </c>
       <c r="C3" s="1">
-        <v>24114</v>
+        <v>24645</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>2.0552396425670187E-2</v>
+        <v>-1.0154346060113728E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,11 +1894,11 @@
         <v>24347</v>
       </c>
       <c r="C4" s="1">
-        <v>23959</v>
+        <v>24514</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>1.5936254980079681E-2</v>
+        <v>-6.8591612929724405E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,11 +1909,11 @@
         <v>22913</v>
       </c>
       <c r="C5" s="1">
-        <v>22709</v>
+        <v>23824</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>8.9032427006502865E-3</v>
+        <v>-3.9759088726923582E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,11 +1924,11 @@
         <v>24664</v>
       </c>
       <c r="C6" s="1">
-        <v>24219</v>
+        <v>24595</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>1.8042491080116768E-2</v>
+        <v>2.7975997405124877E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1933,11 +1939,11 @@
         <v>24906</v>
       </c>
       <c r="C7" s="1">
-        <v>25258</v>
+        <v>25260</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-1.413314060868867E-2</v>
+        <v>-1.421344254396531E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1948,11 +1954,11 @@
         <v>25313</v>
       </c>
       <c r="C8" s="1">
-        <v>25071</v>
+        <v>25796</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>9.5603049816299929E-3</v>
+        <v>-1.9081104570773912E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1963,11 +1969,11 @@
         <v>23366</v>
       </c>
       <c r="C9" s="1">
-        <v>23337</v>
+        <v>23813</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>1.2411195754515108E-3</v>
+        <v>-1.9130360352649148E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1978,11 +1984,11 @@
         <v>24756</v>
       </c>
       <c r="C10" s="1">
-        <v>24365</v>
+        <v>25096</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>1.5794150912910001E-2</v>
+        <v>-1.3734044272095654E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1993,11 +1999,11 @@
         <v>24096</v>
       </c>
       <c r="C11" s="1">
-        <v>24220</v>
+        <v>24744</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>-5.1460823373173968E-3</v>
+        <v>-2.6892430278884463E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2008,11 +2014,11 @@
         <v>42505</v>
       </c>
       <c r="C12" s="1">
-        <v>41351</v>
+        <v>42894</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>2.7149747088577814E-2</v>
+        <v>-9.1518644865309969E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2023,11 +2029,11 @@
         <v>41934</v>
       </c>
       <c r="C13" s="1">
-        <v>40983</v>
+        <v>41668</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>2.267849477750751E-2</v>
+        <v>6.3433013783564651E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2038,11 +2044,11 @@
         <v>41737</v>
       </c>
       <c r="C14" s="1">
-        <v>41417</v>
+        <v>42646</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>7.6670580060857274E-3</v>
+        <v>-2.1779236648537269E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,11 +2059,11 @@
         <v>44801</v>
       </c>
       <c r="C15" s="1">
-        <v>43992</v>
+        <v>45057</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>1.8057632642128525E-2</v>
+        <v>-5.7141581661123639E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2068,11 +2074,11 @@
         <v>42001</v>
       </c>
       <c r="C16" s="1">
-        <v>40717</v>
+        <v>42149</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>3.0570700697602437E-2</v>
+        <v>-3.5237256255803433E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,11 +2089,11 @@
         <v>42946</v>
       </c>
       <c r="C17" s="1">
-        <v>42666</v>
+        <v>43171</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>6.5198155823592415E-3</v>
+        <v>-5.2391375215386764E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2098,11 +2104,11 @@
         <v>41607</v>
       </c>
       <c r="C18" s="1">
-        <v>40661</v>
+        <v>41573</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>2.2736558752133054E-2</v>
+        <v>8.1717018770879901E-4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2113,11 +2119,11 @@
         <v>44441</v>
       </c>
       <c r="C19" s="1">
-        <v>44243</v>
+        <v>45028</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>4.4553452892599175E-3</v>
+        <v>-1.3208523660583695E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2128,11 +2134,11 @@
         <v>43372</v>
       </c>
       <c r="C20" s="1">
-        <v>43664</v>
+        <v>44426</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>-6.7324541178640594E-3</v>
+        <v>-2.4301392603523011E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2143,11 +2149,11 @@
         <v>44275</v>
       </c>
       <c r="C21" s="1">
-        <v>43837</v>
+        <v>44258</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>9.892715979672501E-3</v>
+        <v>3.8396386222473179E-4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2158,11 +2164,11 @@
         <v>60105</v>
       </c>
       <c r="C22" s="1">
-        <v>59910</v>
+        <v>60269</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="0"/>
-        <v>3.2443224357374596E-3</v>
+        <v>-2.7285583562099659E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2173,11 +2179,11 @@
         <v>62231</v>
       </c>
       <c r="C23" s="1">
-        <v>62514</v>
+        <v>62640</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="0"/>
-        <v>-4.5475727531294691E-3</v>
+        <v>-6.5722871237807526E-3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2188,11 +2194,11 @@
         <v>59807</v>
       </c>
       <c r="C24" s="1">
-        <v>59708</v>
+        <v>60089</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="0"/>
-        <v>1.6553246275519589E-3</v>
+        <v>-4.71516712090558E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2203,11 +2209,11 @@
         <v>60379</v>
       </c>
       <c r="C25" s="1">
-        <v>60319</v>
+        <v>60402</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="0"/>
-        <v>9.9372298315639554E-4</v>
+        <v>-3.8092714354328493E-4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,11 +2224,11 @@
         <v>60700</v>
       </c>
       <c r="C26" s="1">
-        <v>61043</v>
+        <v>61104</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="0"/>
-        <v>-5.6507413509060958E-3</v>
+        <v>-6.6556836902800657E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2239,11 @@
         <v>59328</v>
       </c>
       <c r="C27" s="1">
-        <v>58889</v>
+        <v>59292</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="0"/>
-        <v>7.3995415318230855E-3</v>
+        <v>6.0679611650485432E-4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2248,11 +2254,11 @@
         <v>60852</v>
       </c>
       <c r="C28" s="1">
-        <v>60911</v>
+        <v>61559</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="0"/>
-        <v>-9.6956550318806286E-4</v>
+        <v>-1.1618352724643398E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2263,11 +2269,11 @@
         <v>60409</v>
       </c>
       <c r="C29" s="1">
-        <v>61017</v>
+        <v>61495</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="0"/>
-        <v>-1.0064725454816336E-2</v>
+        <v>-1.797745369067523E-2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,11 +2284,11 @@
         <v>59073</v>
       </c>
       <c r="C30" s="1">
-        <v>59146</v>
+        <v>59497</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="0"/>
-        <v>-1.2357591454640869E-3</v>
+        <v>-7.1775599681749699E-3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2293,11 +2299,11 @@
         <v>59972</v>
       </c>
       <c r="C31" s="1">
-        <v>60164</v>
+        <v>60189</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="0"/>
-        <v>-3.2014940305475888E-3</v>
+        <v>-3.618355232441806E-3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -4468,11 +4474,11 @@
         <v>56693</v>
       </c>
       <c r="C212" s="1">
-        <v>54442</v>
+        <v>55199</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>3.970507822835271E-2</v>
+        <v>2.6352459739297621E-2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4483,11 +4489,11 @@
         <v>58318</v>
       </c>
       <c r="C213" s="1">
-        <v>55460</v>
+        <v>54857</v>
       </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>4.9007167598340132E-2</v>
+        <v>5.93470283617408E-2</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
@@ -4498,11 +4504,11 @@
         <v>56553</v>
       </c>
       <c r="C214" s="1">
-        <v>53504</v>
+        <v>53439</v>
       </c>
       <c r="D214" s="2">
         <f t="shared" si="3"/>
-        <v>5.3914027549378456E-2</v>
+        <v>5.5063391862500664E-2</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: add random swap to increase diversity
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B8E3ED-BEF0-405B-BB78-4998CE22E101}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9954EC-DC14-4CC4-A0B5-342037757B9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="1770" windowWidth="14070" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="best-feasible-slns" sheetId="1" r:id="rId1"/>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1860,15 +1860,15 @@
         <v>24038</v>
       </c>
       <c r="C2" s="1">
-        <v>24373</v>
+        <v>24281</v>
       </c>
       <c r="D2" s="2">
         <f>(B2-C2)/B2</f>
-        <v>-1.3936267576337466E-2</v>
+        <v>-1.010899409268658E-2</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(D2:D31)</f>
-        <v>-9.6011628899455824E-3</v>
+        <v>-8.8053169176028935E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1879,11 +1879,11 @@
         <v>24620</v>
       </c>
       <c r="C3" s="1">
-        <v>24645</v>
+        <v>24745</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D66" si="0">(B3-C3)/B3</f>
-        <v>-1.0154346060113728E-3</v>
+        <v>-5.077173030056864E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1894,11 +1894,11 @@
         <v>24347</v>
       </c>
       <c r="C4" s="1">
-        <v>24514</v>
+        <v>24379</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>-6.8591612929724405E-3</v>
+        <v>-1.3143303076354376E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1909,11 +1909,11 @@
         <v>22913</v>
       </c>
       <c r="C5" s="1">
-        <v>23824</v>
+        <v>23520</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>-3.9759088726923582E-2</v>
+        <v>-2.649151136909178E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1939,11 +1939,11 @@
         <v>24906</v>
       </c>
       <c r="C7" s="1">
-        <v>25260</v>
+        <v>25448</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>-1.421344254396531E-2</v>
+        <v>-2.1761824459969485E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1969,11 +1969,11 @@
         <v>23366</v>
       </c>
       <c r="C9" s="1">
-        <v>23813</v>
+        <v>23835</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>-1.9130360352649148E-2</v>
+        <v>-2.0071899340922707E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1999,11 +1999,11 @@
         <v>24096</v>
       </c>
       <c r="C11" s="1">
-        <v>24744</v>
+        <v>24679</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>-2.6892430278884463E-2</v>
+        <v>-2.419488711819389E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2014,11 +2014,11 @@
         <v>42505</v>
       </c>
       <c r="C12" s="1">
-        <v>42894</v>
+        <v>42787</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>-9.1518644865309969E-3</v>
+        <v>-6.6345135866368666E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2029,11 +2029,11 @@
         <v>41934</v>
       </c>
       <c r="C13" s="1">
-        <v>41668</v>
+        <v>42260</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>6.3433013783564651E-3</v>
+        <v>-7.7741212381361186E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2044,11 +2044,11 @@
         <v>41737</v>
       </c>
       <c r="C14" s="1">
-        <v>42646</v>
+        <v>41342</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>-2.1779236648537269E-2</v>
+        <v>9.4640247262620693E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2059,11 +2059,11 @@
         <v>44801</v>
       </c>
       <c r="C15" s="1">
-        <v>45057</v>
+        <v>45309</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>-5.7141581661123639E-3</v>
+        <v>-1.1339032610879221E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2074,11 +2074,11 @@
         <v>42001</v>
       </c>
       <c r="C16" s="1">
-        <v>42149</v>
+        <v>42272</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>-3.5237256255803433E-3</v>
+        <v>-6.4522273279207639E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4474,11 +4474,11 @@
         <v>56693</v>
       </c>
       <c r="C212" s="1">
-        <v>55199</v>
+        <v>55391</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>2.6352459739297621E-2</v>
+        <v>2.2965798246697124E-2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4489,11 +4489,11 @@
         <v>58318</v>
       </c>
       <c r="C213" s="1">
-        <v>54857</v>
+        <v>56741</v>
       </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>5.93470283617408E-2</v>
+        <v>2.7041393737782502E-2</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
@@ -4504,11 +4504,11 @@
         <v>56553</v>
       </c>
       <c r="C214" s="1">
-        <v>53439</v>
+        <v>54216</v>
       </c>
       <c r="D214" s="2">
         <f t="shared" si="3"/>
-        <v>5.5063391862500664E-2</v>
+        <v>4.1324067688716777E-2</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
docs: final verion 1
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659109C1-FB60-4BCB-BDFE-DDBF536061DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512801C7-43E8-4F45-9A1D-282C5E190DC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1828,7 +1828,7 @@
   <dimension ref="A1:E546"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="C212" sqref="C212:C241"/>
+      <selection activeCell="I220" sqref="I220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4474,11 +4474,11 @@
         <v>56693</v>
       </c>
       <c r="C212">
-        <v>55416</v>
+        <v>55302</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>2.2524826698181434E-2</v>
+        <v>2.4535656959412979E-2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: final version v2
change random swap back to VNS
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512801C7-43E8-4F45-9A1D-282C5E190DC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6DEA60-E299-41F6-A437-18B639AF0E48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="I220" sqref="I220"/>
+    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+      <selection activeCell="C212" sqref="C212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4474,11 +4474,11 @@
         <v>56693</v>
       </c>
       <c r="C212">
-        <v>55302</v>
+        <v>55979</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>2.4535656959412979E-2</v>
+        <v>1.2594147425608099E-2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4489,11 +4489,11 @@
         <v>58318</v>
       </c>
       <c r="C213">
-        <v>57021</v>
+        <v>57468</v>
       </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>2.2240131691758976E-2</v>
+        <v>1.4575259782571419E-2</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
@@ -4504,11 +4504,11 @@
         <v>56553</v>
       </c>
       <c r="C214">
-        <v>55387</v>
+        <v>54878</v>
       </c>
       <c r="D214" s="2">
         <f t="shared" si="3"/>
-        <v>2.061782752462292E-2</v>
+        <v>2.9618234222764488E-2</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
@@ -4519,11 +4519,11 @@
         <v>56863</v>
       </c>
       <c r="C215">
-        <v>55451</v>
+        <v>56076</v>
       </c>
       <c r="D215" s="2">
         <f t="shared" si="3"/>
-        <v>2.4831612823804583E-2</v>
+        <v>1.3840282784939239E-2</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
@@ -4534,11 +4534,11 @@
         <v>56629</v>
       </c>
       <c r="C216">
-        <v>55163</v>
+        <v>55567</v>
       </c>
       <c r="D216" s="2">
         <f t="shared" si="3"/>
-        <v>2.588779600558018E-2</v>
+        <v>1.8753642126825478E-2</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
@@ -4549,11 +4549,11 @@
         <v>57119</v>
       </c>
       <c r="C217">
-        <v>55969</v>
+        <v>56214</v>
       </c>
       <c r="D217" s="2">
         <f t="shared" si="3"/>
-        <v>2.0133405696878447E-2</v>
+        <v>1.5844114917978255E-2</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
@@ -4564,11 +4564,11 @@
         <v>56292</v>
       </c>
       <c r="C218">
-        <v>55105</v>
+        <v>54791</v>
       </c>
       <c r="D218" s="2">
         <f t="shared" si="3"/>
-        <v>2.1086477652241881E-2</v>
+        <v>2.6664534925033751E-2</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
@@ -4579,11 +4579,11 @@
         <v>56403</v>
       </c>
       <c r="C219">
-        <v>55114</v>
+        <v>54987</v>
       </c>
       <c r="D219" s="2">
         <f t="shared" si="3"/>
-        <v>2.2853394322997003E-2</v>
+        <v>2.510504760385086E-2</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
@@ -4594,11 +4594,11 @@
         <v>57442</v>
       </c>
       <c r="C220">
-        <v>56019</v>
+        <v>55285</v>
       </c>
       <c r="D220" s="2">
         <f t="shared" si="3"/>
-        <v>2.4772814317050241E-2</v>
+        <v>3.7550920928937012E-2</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
@@ -4609,11 +4609,11 @@
         <v>56447</v>
       </c>
       <c r="C221">
-        <v>54503</v>
+        <v>55116</v>
       </c>
       <c r="D221" s="2">
         <f t="shared" si="3"/>
-        <v>3.4439385618367672E-2</v>
+        <v>2.3579641079242476E-2</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
@@ -4624,11 +4624,11 @@
         <v>107689</v>
       </c>
       <c r="C222">
-        <v>106952</v>
+        <v>106953</v>
       </c>
       <c r="D222" s="2">
         <f t="shared" si="3"/>
-        <v>6.8437816304357923E-3</v>
+        <v>6.8344956309372359E-3</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
@@ -4639,11 +4639,11 @@
         <v>108338</v>
       </c>
       <c r="C223">
-        <v>107695</v>
+        <v>107224</v>
       </c>
       <c r="D223" s="2">
         <f t="shared" si="3"/>
-        <v>5.935128948291458E-3</v>
+        <v>1.0282633978843988E-2</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
@@ -4654,11 +4654,11 @@
         <v>106385</v>
       </c>
       <c r="C224">
-        <v>104850</v>
+        <v>105175</v>
       </c>
       <c r="D224" s="2">
         <f t="shared" si="3"/>
-        <v>1.442872585420877E-2</v>
+        <v>1.1373783898105935E-2</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
@@ -4669,11 +4669,11 @@
         <v>106796</v>
       </c>
       <c r="C225">
-        <v>105469</v>
+        <v>106131</v>
       </c>
       <c r="D225" s="2">
         <f t="shared" si="3"/>
-        <v>1.2425559009700738E-2</v>
+        <v>6.226824974718154E-3</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
@@ -4684,11 +4684,11 @@
         <v>107396</v>
       </c>
       <c r="C226">
-        <v>106639</v>
+        <v>106369</v>
       </c>
       <c r="D226" s="2">
         <f t="shared" si="3"/>
-        <v>7.0486796528734779E-3</v>
+        <v>9.5627397668442034E-3</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
@@ -4699,11 +4699,11 @@
         <v>107246</v>
       </c>
       <c r="C227">
-        <v>105764</v>
+        <v>106226</v>
       </c>
       <c r="D227" s="2">
         <f t="shared" si="3"/>
-        <v>1.3818697200828003E-2</v>
+        <v>9.5108442272905276E-3</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
@@ -4714,11 +4714,11 @@
         <v>106308</v>
       </c>
       <c r="C228">
-        <v>105387</v>
+        <v>105504</v>
       </c>
       <c r="D228" s="2">
         <f t="shared" si="3"/>
-        <v>8.6635060390563273E-3</v>
+        <v>7.562930353313015E-3</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
@@ -4729,11 +4729,11 @@
         <v>103993</v>
       </c>
       <c r="C229">
-        <v>102951</v>
+        <v>103098</v>
       </c>
       <c r="D229" s="2">
         <f t="shared" si="3"/>
-        <v>1.0019905185925975E-2</v>
+        <v>8.6063485042262456E-3</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
@@ -4744,11 +4744,11 @@
         <v>106835</v>
       </c>
       <c r="C230">
-        <v>105957</v>
+        <v>106040</v>
       </c>
       <c r="D230" s="2">
         <f t="shared" si="3"/>
-        <v>8.2182805260448358E-3</v>
+        <v>7.441381569710301E-3</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
@@ -4759,11 +4759,11 @@
         <v>105751</v>
       </c>
       <c r="C231">
-        <v>104838</v>
+        <v>104829</v>
       </c>
       <c r="D231" s="2">
         <f t="shared" si="3"/>
-        <v>8.6334880994033154E-3</v>
+        <v>8.7185936776011577E-3</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
@@ -4774,11 +4774,11 @@
         <v>150083</v>
       </c>
       <c r="C232">
-        <v>149612</v>
+        <v>149534</v>
       </c>
       <c r="D232" s="2">
         <f t="shared" si="3"/>
-        <v>3.138263494199876E-3</v>
+        <v>3.6579759199909384E-3</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
@@ -4789,11 +4789,11 @@
         <v>149907</v>
       </c>
       <c r="C233">
-        <v>149622</v>
+        <v>149610</v>
       </c>
       <c r="D233" s="2">
         <f t="shared" si="3"/>
-        <v>1.9011787308131042E-3</v>
+        <v>1.9812283615841821E-3</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
@@ -4804,11 +4804,11 @@
         <v>152993</v>
       </c>
       <c r="C234">
-        <v>152304</v>
+        <v>152338</v>
       </c>
       <c r="D234" s="2">
         <f t="shared" si="3"/>
-        <v>4.5034740151510197E-3</v>
+        <v>4.2812416254338435E-3</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
@@ -4819,11 +4819,11 @@
         <v>153169</v>
       </c>
       <c r="C235">
-        <v>152723</v>
+        <v>152477</v>
       </c>
       <c r="D235" s="2">
         <f t="shared" si="3"/>
-        <v>2.9118163597072516E-3</v>
+        <v>4.517885472909009E-3</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
@@ -4834,11 +4834,11 @@
         <v>150287</v>
       </c>
       <c r="C236">
-        <v>149638</v>
+        <v>149768</v>
       </c>
       <c r="D236" s="2">
         <f t="shared" si="3"/>
-        <v>4.3184041201168432E-3</v>
+        <v>3.4533925089994476E-3</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
@@ -4849,11 +4849,11 @@
         <v>148544</v>
       </c>
       <c r="C237">
-        <v>147863</v>
+        <v>147611</v>
       </c>
       <c r="D237" s="2">
         <f t="shared" si="3"/>
-        <v>4.5845002154243858E-3</v>
+        <v>6.280967255493322E-3</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
@@ -4864,11 +4864,11 @@
         <v>147471</v>
       </c>
       <c r="C238">
-        <v>146429</v>
+        <v>146680</v>
       </c>
       <c r="D238" s="2">
         <f t="shared" si="3"/>
-        <v>7.0657959870076151E-3</v>
+        <v>5.3637664354347636E-3</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
@@ -4879,11 +4879,11 @@
         <v>152841</v>
       </c>
       <c r="C239">
-        <v>152189</v>
+        <v>151631</v>
       </c>
       <c r="D239" s="2">
         <f t="shared" si="3"/>
-        <v>4.2658710686268734E-3</v>
+        <v>7.9167239157032464E-3</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
@@ -4894,11 +4894,11 @@
         <v>149568</v>
       </c>
       <c r="C240">
-        <v>149032</v>
+        <v>148550</v>
       </c>
       <c r="D240" s="2">
         <f t="shared" si="3"/>
-        <v>3.5836542575952077E-3</v>
+        <v>6.8062687205819429E-3</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
@@ -4909,11 +4909,11 @@
         <v>149572</v>
       </c>
       <c r="C241">
-        <v>148348</v>
+        <v>148560</v>
       </c>
       <c r="D241" s="2">
         <f t="shared" si="3"/>
-        <v>8.1833498248335256E-3</v>
+        <v>6.7659722407937316E-3</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: correct update global best in VNS
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6DEA60-E299-41F6-A437-18B639AF0E48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4BEB0A-5E60-4092-8240-9737CB9CBB1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1828,7 +1828,7 @@
   <dimension ref="A1:E546"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="C212" sqref="C212"/>
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4474,11 +4474,11 @@
         <v>56693</v>
       </c>
       <c r="C212">
-        <v>55979</v>
+        <v>55480</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>1.2594147425608099E-2</v>
+        <v>2.1395939533981268E-2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4489,11 +4489,11 @@
         <v>58318</v>
       </c>
       <c r="C213">
-        <v>57468</v>
+        <v>57341</v>
       </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>1.4575259782571419E-2</v>
+        <v>1.6752975067732091E-2</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: add random select after VNS
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4BEB0A-5E60-4092-8240-9737CB9CBB1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19B0F7A-7409-44F6-96E0-1DFF744004C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="K215" sqref="K215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4474,11 +4474,11 @@
         <v>56693</v>
       </c>
       <c r="C212">
-        <v>55480</v>
+        <v>55967</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>2.1395939533981268E-2</v>
+        <v>1.280581376889563E-2</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: final version before free memory
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19B0F7A-7409-44F6-96E0-1DFF744004C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1A0DAD-8CFC-468C-B746-9A0ECD23AB69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="K215" sqref="K215"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="62" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3753,9 +3753,12 @@
       <c r="B152" s="1">
         <v>117726</v>
       </c>
+      <c r="C152" s="1">
+        <v>116981</v>
+      </c>
       <c r="D152" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6.3282537417392931E-3</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -3765,9 +3768,12 @@
       <c r="B153" s="1">
         <v>119139</v>
       </c>
+      <c r="C153" s="1">
+        <v>118857</v>
+      </c>
       <c r="D153" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.3669831037695464E-3</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -4474,11 +4480,11 @@
         <v>56693</v>
       </c>
       <c r="C212">
-        <v>55967</v>
+        <v>56374</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>1.280581376889563E-2</v>
+        <v>5.6267969590602018E-3</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4489,11 +4495,11 @@
         <v>58318</v>
       </c>
       <c r="C213">
-        <v>57341</v>
+        <v>57962</v>
       </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>1.6752975067732091E-2</v>
+        <v>6.1044617442299115E-3</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
@@ -4504,11 +4510,11 @@
         <v>56553</v>
       </c>
       <c r="C214">
-        <v>54878</v>
+        <v>56291</v>
       </c>
       <c r="D214" s="2">
         <f t="shared" si="3"/>
-        <v>2.9618234222764488E-2</v>
+        <v>4.6328223082771911E-3</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
@@ -4519,11 +4525,11 @@
         <v>56863</v>
       </c>
       <c r="C215">
-        <v>56076</v>
+        <v>56563</v>
       </c>
       <c r="D215" s="2">
         <f t="shared" si="3"/>
-        <v>1.3840282784939239E-2</v>
+        <v>5.2758384186553644E-3</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
@@ -4534,11 +4540,11 @@
         <v>56629</v>
       </c>
       <c r="C216">
-        <v>55567</v>
+        <v>56279</v>
       </c>
       <c r="D216" s="2">
         <f t="shared" si="3"/>
-        <v>1.8753642126825478E-2</v>
+        <v>6.1805788553567957E-3</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
@@ -4549,11 +4555,11 @@
         <v>57119</v>
       </c>
       <c r="C217">
-        <v>56214</v>
+        <v>56814</v>
       </c>
       <c r="D217" s="2">
         <f t="shared" si="3"/>
-        <v>1.5844114917978255E-2</v>
+        <v>5.3397293369981964E-3</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
@@ -4564,11 +4570,11 @@
         <v>56292</v>
       </c>
       <c r="C218">
-        <v>54791</v>
+        <v>55769</v>
       </c>
       <c r="D218" s="2">
         <f t="shared" si="3"/>
-        <v>2.6664534925033751E-2</v>
+        <v>9.290840616783912E-3</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
@@ -4579,11 +4585,11 @@
         <v>56403</v>
       </c>
       <c r="C219">
-        <v>54987</v>
+        <v>56079</v>
       </c>
       <c r="D219" s="2">
         <f t="shared" si="3"/>
-        <v>2.510504760385086E-2</v>
+        <v>5.7443752991862135E-3</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
@@ -4594,11 +4600,11 @@
         <v>57442</v>
       </c>
       <c r="C220">
-        <v>55285</v>
+        <v>56873</v>
       </c>
       <c r="D220" s="2">
         <f t="shared" si="3"/>
-        <v>3.7550920928937012E-2</v>
+        <v>9.9056439539013264E-3</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
@@ -4609,11 +4615,11 @@
         <v>56447</v>
       </c>
       <c r="C221">
-        <v>55116</v>
+        <v>55951</v>
       </c>
       <c r="D221" s="2">
         <f t="shared" si="3"/>
-        <v>2.3579641079242476E-2</v>
+        <v>8.7870037380197354E-3</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
@@ -4624,11 +4630,11 @@
         <v>107689</v>
       </c>
       <c r="C222">
-        <v>106953</v>
+        <v>107247</v>
       </c>
       <c r="D222" s="2">
         <f t="shared" si="3"/>
-        <v>6.8344956309372359E-3</v>
+        <v>4.1044117783617636E-3</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
@@ -4639,11 +4645,11 @@
         <v>108338</v>
       </c>
       <c r="C223">
-        <v>107224</v>
+        <v>107679</v>
       </c>
       <c r="D223" s="2">
         <f t="shared" si="3"/>
-        <v>1.0282633978843988E-2</v>
+        <v>6.082814894127638E-3</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
@@ -4654,11 +4660,11 @@
         <v>106385</v>
       </c>
       <c r="C224">
-        <v>105175</v>
+        <v>105989</v>
       </c>
       <c r="D224" s="2">
         <f t="shared" si="3"/>
-        <v>1.1373783898105935E-2</v>
+        <v>3.7223292757437611E-3</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
@@ -4669,11 +4675,11 @@
         <v>106796</v>
       </c>
       <c r="C225">
-        <v>106131</v>
+        <v>106215</v>
       </c>
       <c r="D225" s="2">
         <f t="shared" si="3"/>
-        <v>6.226824974718154E-3</v>
+        <v>5.4402786621221772E-3</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
@@ -4684,11 +4690,11 @@
         <v>107396</v>
       </c>
       <c r="C226">
-        <v>106369</v>
+        <v>106880</v>
       </c>
       <c r="D226" s="2">
         <f t="shared" si="3"/>
-        <v>9.5627397668442034E-3</v>
+        <v>4.804648217810719E-3</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
@@ -4699,11 +4705,11 @@
         <v>107246</v>
       </c>
       <c r="C227">
-        <v>106226</v>
+        <v>106726</v>
       </c>
       <c r="D227" s="2">
         <f t="shared" si="3"/>
-        <v>9.5108442272905276E-3</v>
+        <v>4.8486656845010533E-3</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
@@ -4714,11 +4720,11 @@
         <v>106308</v>
       </c>
       <c r="C228">
-        <v>105504</v>
+        <v>105880</v>
       </c>
       <c r="D228" s="2">
         <f t="shared" si="3"/>
-        <v>7.562930353313015E-3</v>
+        <v>4.0260375512661322E-3</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
@@ -4729,11 +4735,11 @@
         <v>103993</v>
       </c>
       <c r="C229">
-        <v>103098</v>
+        <v>103667</v>
       </c>
       <c r="D229" s="2">
         <f t="shared" si="3"/>
-        <v>8.6063485042262456E-3</v>
+        <v>3.134826382544979E-3</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
@@ -4744,11 +4750,11 @@
         <v>106835</v>
       </c>
       <c r="C230">
-        <v>106040</v>
+        <v>106280</v>
       </c>
       <c r="D230" s="2">
         <f t="shared" si="3"/>
-        <v>7.441381569710301E-3</v>
+        <v>5.1949267562128518E-3</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
@@ -4759,11 +4765,11 @@
         <v>105751</v>
       </c>
       <c r="C231">
-        <v>104829</v>
+        <v>105409</v>
       </c>
       <c r="D231" s="2">
         <f t="shared" si="3"/>
-        <v>8.7185936776011577E-3</v>
+        <v>3.2340119715179999E-3</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
@@ -4774,11 +4780,11 @@
         <v>150083</v>
       </c>
       <c r="C232">
-        <v>149534</v>
+        <v>149885</v>
       </c>
       <c r="D232" s="2">
         <f t="shared" si="3"/>
-        <v>3.6579759199909384E-3</v>
+        <v>1.3192700039311581E-3</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
@@ -4789,11 +4795,11 @@
         <v>149907</v>
       </c>
       <c r="C233">
-        <v>149610</v>
+        <v>149616</v>
       </c>
       <c r="D233" s="2">
         <f t="shared" si="3"/>
-        <v>1.9812283615841821E-3</v>
+        <v>1.9412035461986432E-3</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
@@ -4804,11 +4810,11 @@
         <v>152993</v>
       </c>
       <c r="C234">
-        <v>152338</v>
+        <v>152610</v>
       </c>
       <c r="D234" s="2">
         <f t="shared" si="3"/>
-        <v>4.2812416254338435E-3</v>
+        <v>2.5033825076964306E-3</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.3">
@@ -4819,11 +4825,11 @@
         <v>153169</v>
       </c>
       <c r="C235">
-        <v>152477</v>
+        <v>152826</v>
       </c>
       <c r="D235" s="2">
         <f t="shared" si="3"/>
-        <v>4.517885472909009E-3</v>
+        <v>2.239356527756922E-3</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
@@ -4834,11 +4840,11 @@
         <v>150287</v>
       </c>
       <c r="C236">
-        <v>149768</v>
+        <v>150115</v>
       </c>
       <c r="D236" s="2">
         <f t="shared" si="3"/>
-        <v>3.4533925089994476E-3</v>
+        <v>1.1444769008630154E-3</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
@@ -4849,11 +4855,11 @@
         <v>148544</v>
       </c>
       <c r="C237">
-        <v>147611</v>
+        <v>148038</v>
       </c>
       <c r="D237" s="2">
         <f t="shared" si="3"/>
-        <v>6.280967255493322E-3</v>
+        <v>3.4063981042654029E-3</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
@@ -4864,11 +4870,11 @@
         <v>147471</v>
       </c>
       <c r="C238">
-        <v>146680</v>
+        <v>147215</v>
       </c>
       <c r="D238" s="2">
         <f t="shared" si="3"/>
-        <v>5.3637664354347636E-3</v>
+        <v>1.7359345227197212E-3</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
@@ -4879,11 +4885,11 @@
         <v>152841</v>
       </c>
       <c r="C239">
-        <v>151631</v>
+        <v>152591</v>
       </c>
       <c r="D239" s="2">
         <f t="shared" si="3"/>
-        <v>7.9167239157032464E-3</v>
+        <v>1.6356867594428197E-3</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
@@ -4894,11 +4900,11 @@
         <v>149568</v>
       </c>
       <c r="C240">
-        <v>148550</v>
+        <v>149351</v>
       </c>
       <c r="D240" s="2">
         <f t="shared" si="3"/>
-        <v>6.8062687205819429E-3</v>
+        <v>1.4508451005562687E-3</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
@@ -4909,11 +4915,11 @@
         <v>149572</v>
       </c>
       <c r="C241">
-        <v>148560</v>
+        <v>149294</v>
       </c>
       <c r="D241" s="2">
         <f t="shared" si="3"/>
-        <v>6.7659722407937316E-3</v>
+        <v>1.8586366432219933E-3</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: add repair after VNS
</commit_message>
<xml_diff>
--- a/gap calculate.xlsx
+++ b/gap calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNNC\Y3_spring\AIM\CW\cw\code\git\AIM_CW_PSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1A0DAD-8CFC-468C-B746-9A0ECD23AB69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FB8EC1-FE3F-454F-A780-DAEA393B8C0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="62" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3754,11 +3754,11 @@
         <v>117726</v>
       </c>
       <c r="C152" s="1">
-        <v>116981</v>
+        <v>117075</v>
       </c>
       <c r="D152" s="2">
         <f t="shared" si="2"/>
-        <v>6.3282537417392931E-3</v>
+        <v>5.5297895112379593E-3</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -3769,11 +3769,11 @@
         <v>119139</v>
       </c>
       <c r="C153" s="1">
-        <v>118857</v>
+        <v>118521</v>
       </c>
       <c r="D153" s="2">
         <f t="shared" si="2"/>
-        <v>2.3669831037695464E-3</v>
+        <v>5.1872182912396448E-3</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -3783,9 +3783,12 @@
       <c r="B154" s="1">
         <v>119159</v>
       </c>
+      <c r="C154" s="1">
+        <v>118270</v>
+      </c>
       <c r="D154" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7.4606198440738845E-3</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -3795,9 +3798,12 @@
       <c r="B155" s="1">
         <v>118802</v>
       </c>
+      <c r="C155" s="1">
+        <v>118063</v>
+      </c>
       <c r="D155" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6.2204339994276188E-3</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -3807,9 +3813,12 @@
       <c r="B156" s="1">
         <v>116434</v>
       </c>
+      <c r="C156" s="1">
+        <v>115355</v>
+      </c>
       <c r="D156" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9.2670525791435487E-3</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
@@ -3819,9 +3828,12 @@
       <c r="B157" s="1">
         <v>119454</v>
       </c>
+      <c r="C157" s="1">
+        <v>118572</v>
+      </c>
       <c r="D157" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7.383595358882917E-3</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -3831,9 +3843,12 @@
       <c r="B158" s="1">
         <v>119749</v>
       </c>
+      <c r="C158" s="1">
+        <v>119139</v>
+      </c>
       <c r="D158" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5.0939882587746031E-3</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
@@ -3843,9 +3858,12 @@
       <c r="B159" s="1">
         <v>118288</v>
       </c>
+      <c r="C159" s="1">
+        <v>117480</v>
+      </c>
       <c r="D159" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>6.8307858785337482E-3</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -3855,9 +3873,12 @@
       <c r="B160" s="1">
         <v>117779</v>
       </c>
+      <c r="C160" s="1">
+        <v>116904</v>
+      </c>
       <c r="D160" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7.4291681878772952E-3</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -3867,9 +3888,12 @@
       <c r="B161" s="1">
         <v>119125</v>
       </c>
+      <c r="C161" s="1">
+        <v>118028</v>
+      </c>
       <c r="D161" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9.2088142707240292E-3</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
@@ -3879,9 +3903,12 @@
       <c r="B162" s="1">
         <v>217318</v>
       </c>
+      <c r="C162" s="1">
+        <v>216414</v>
+      </c>
       <c r="D162" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.1598026854655391E-3</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -3891,9 +3918,12 @@
       <c r="B163" s="1">
         <v>219022</v>
       </c>
+      <c r="C163" s="1">
+        <v>217799</v>
+      </c>
       <c r="D163" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5.5839139447178823E-3</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -3903,9 +3933,12 @@
       <c r="B164" s="1">
         <v>217772</v>
       </c>
+      <c r="C164" s="1">
+        <v>216809</v>
+      </c>
       <c r="D164" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.4220560953657957E-3</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
@@ -3915,9 +3948,12 @@
       <c r="B165" s="1">
         <v>216802</v>
       </c>
+      <c r="C165" s="1">
+        <v>216375</v>
+      </c>
       <c r="D165" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.9695390263927454E-3</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
@@ -3927,9 +3963,12 @@
       <c r="B166" s="1">
         <v>213809</v>
       </c>
+      <c r="C166" s="1">
+        <v>212714</v>
+      </c>
       <c r="D166" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5.1213933931686696E-3</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
@@ -3939,9 +3978,12 @@
       <c r="B167" s="1">
         <v>215013</v>
       </c>
+      <c r="C167" s="1">
+        <v>213816</v>
+      </c>
       <c r="D167" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5.5671052447991516E-3</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
@@ -3951,9 +3993,12 @@
       <c r="B168" s="1">
         <v>217896</v>
       </c>
+      <c r="C168" s="1">
+        <v>217089</v>
+      </c>
       <c r="D168" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.7036017182509088E-3</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -3963,9 +4008,12 @@
       <c r="B169" s="1">
         <v>219949</v>
       </c>
+      <c r="C169" s="1">
+        <v>219148</v>
+      </c>
       <c r="D169" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.6417533155413302E-3</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
@@ -3975,9 +4023,12 @@
       <c r="B170" s="1">
         <v>214332</v>
       </c>
+      <c r="C170" s="1">
+        <v>213129</v>
+      </c>
       <c r="D170" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5.6127876378702203E-3</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
@@ -3987,9 +4038,12 @@
       <c r="B171" s="1">
         <v>220833</v>
       </c>
+      <c r="C171" s="1">
+        <v>220081</v>
+      </c>
       <c r="D171" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.4052881589255227E-3</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
@@ -3999,9 +4053,12 @@
       <c r="B172" s="1">
         <v>304344</v>
       </c>
+      <c r="C172" s="1">
+        <v>303626</v>
+      </c>
       <c r="D172" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.3591725153116212E-3</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
@@ -4011,9 +4068,12 @@
       <c r="B173" s="1">
         <v>302332</v>
       </c>
+      <c r="C173" s="1">
+        <v>301811</v>
+      </c>
       <c r="D173" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.7232711059365202E-3</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -4023,9 +4083,12 @@
       <c r="B174" s="1">
         <v>302354</v>
       </c>
+      <c r="C174" s="1">
+        <v>301895</v>
+      </c>
       <c r="D174" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.5180880689522878E-3</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -4035,9 +4098,12 @@
       <c r="B175" s="1">
         <v>300743</v>
       </c>
+      <c r="C175" s="1">
+        <v>300423</v>
+      </c>
       <c r="D175" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0640314155275434E-3</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -4047,9 +4113,12 @@
       <c r="B176" s="1">
         <v>304344</v>
       </c>
+      <c r="C176" s="1">
+        <v>304011</v>
+      </c>
       <c r="D176" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0941566122545541E-3</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -4059,9 +4128,12 @@
       <c r="B177" s="1">
         <v>301730</v>
       </c>
+      <c r="C177" s="1">
+        <v>301042</v>
+      </c>
       <c r="D177" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.2801842707055979E-3</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
@@ -4071,9 +4143,12 @@
       <c r="B178" s="1">
         <v>304949</v>
       </c>
+      <c r="C178" s="1">
+        <v>304514</v>
+      </c>
       <c r="D178" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.4264680323595093E-3</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
@@ -4083,9 +4158,12 @@
       <c r="B179" s="1">
         <v>296437</v>
       </c>
+      <c r="C179" s="1">
+        <v>295195</v>
+      </c>
       <c r="D179" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.1897603875359684E-3</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
@@ -4095,9 +4173,12 @@
       <c r="B180" s="1">
         <v>301313</v>
       </c>
+      <c r="C180" s="1">
+        <v>300773</v>
+      </c>
       <c r="D180" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.7921563291328287E-3</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -4107,9 +4188,12 @@
       <c r="B181" s="1">
         <v>307014</v>
       </c>
+      <c r="C181" s="1">
+        <v>306622</v>
+      </c>
       <c r="D181" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.2768147380901197E-3</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -4119,9 +4203,12 @@
       <c r="B182" s="1">
         <v>21946</v>
       </c>
+      <c r="C182" s="1">
+        <v>21772</v>
+      </c>
       <c r="D182" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7.9285519001184718E-3</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -4131,9 +4218,12 @@
       <c r="B183" s="1">
         <v>21716</v>
       </c>
+      <c r="C183" s="1">
+        <v>21492</v>
+      </c>
       <c r="D183" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0314975133542089E-2</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -4143,9 +4233,12 @@
       <c r="B184" s="1">
         <v>20754</v>
       </c>
+      <c r="C184" s="1">
+        <v>20675</v>
+      </c>
       <c r="D184" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.8064951334682469E-3</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
@@ -4155,9 +4248,12 @@
       <c r="B185" s="1">
         <v>21464</v>
       </c>
+      <c r="C185" s="1">
+        <v>21411</v>
+      </c>
       <c r="D185" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.4692508386134925E-3</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -4167,9 +4263,12 @@
       <c r="B186" s="1">
         <v>21814</v>
       </c>
+      <c r="C186" s="1">
+        <v>21733</v>
+      </c>
       <c r="D186" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3.7132116989089577E-3</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
@@ -4179,9 +4278,12 @@
       <c r="B187" s="1">
         <v>22176</v>
       </c>
+      <c r="C187" s="1">
+        <v>22176</v>
+      </c>
       <c r="D187" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
@@ -4191,9 +4293,12 @@
       <c r="B188" s="1">
         <v>21799</v>
       </c>
+      <c r="C188" s="1">
+        <v>21699</v>
+      </c>
       <c r="D188" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.5873663929538056E-3</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
@@ -4203,9 +4308,12 @@
       <c r="B189" s="1">
         <v>21397</v>
       </c>
+      <c r="C189" s="1">
+        <v>21169</v>
+      </c>
       <c r="D189" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0655699397111744E-2</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
@@ -4215,9 +4323,12 @@
       <c r="B190" s="1">
         <v>22493</v>
       </c>
+      <c r="C190" s="1">
+        <v>22386</v>
+      </c>
       <c r="D190" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.7570355221624502E-3</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -4227,9 +4338,12 @@
       <c r="B191" s="1">
         <v>20983</v>
       </c>
+      <c r="C191" s="1">
+        <v>20944</v>
+      </c>
       <c r="D191" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.8586474765286184E-3</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
@@ -4239,9 +4353,12 @@
       <c r="B192" s="1">
         <v>40767</v>
       </c>
+      <c r="C192" s="1">
+        <v>40575</v>
+      </c>
       <c r="D192" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.7096916623739788E-3</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
@@ -4251,9 +4368,12 @@
       <c r="B193" s="1">
         <v>41304</v>
       </c>
+      <c r="C193" s="1">
+        <v>41199</v>
+      </c>
       <c r="D193" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.5421266705403837E-3</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
@@ -4263,9 +4383,12 @@
       <c r="B194" s="1">
         <v>41560</v>
       </c>
+      <c r="C194" s="1">
+        <v>41473</v>
+      </c>
       <c r="D194" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.0933589990375359E-3</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
@@ -4275,9 +4398,12 @@
       <c r="B195" s="1">
         <v>41041</v>
       </c>
+      <c r="C195" s="1">
+        <v>40972</v>
+      </c>
       <c r="D195" s="2">
         <f t="shared" ref="D195:D258" si="3">(B195-C195)/B195</f>
-        <v>1</v>
+        <v>1.6812455836846081E-3</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
@@ -4287,9 +4413,12 @@
       <c r="B196" s="1">
         <v>40872</v>
       </c>
+      <c r="C196" s="1">
+        <v>40872</v>
+      </c>
       <c r="D196" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
@@ -4299,9 +4428,12 @@
       <c r="B197" s="1">
         <v>41058</v>
       </c>
+      <c r="C197" s="1">
+        <v>41058</v>
+      </c>
       <c r="D197" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
@@ -4311,9 +4443,12 @@
       <c r="B198" s="1">
         <v>41062</v>
       </c>
+      <c r="C198" s="1">
+        <v>40887</v>
+      </c>
       <c r="D198" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4.2618479372655985E-3</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
@@ -4323,9 +4458,12 @@
       <c r="B199" s="1">
         <v>42719</v>
       </c>
+      <c r="C199" s="1">
+        <v>42719</v>
+      </c>
       <c r="D199" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
@@ -4335,9 +4473,12 @@
       <c r="B200" s="1">
         <v>42230</v>
       </c>
+      <c r="C200" s="1">
+        <v>42230</v>
+      </c>
       <c r="D200" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
@@ -4347,9 +4488,12 @@
       <c r="B201" s="1">
         <v>41700</v>
       </c>
+      <c r="C201" s="1">
+        <v>41524</v>
+      </c>
       <c r="D201" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4.2206235011990403E-3</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
@@ -4359,9 +4503,12 @@
       <c r="B202" s="1">
         <v>57494</v>
       </c>
+      <c r="C202" s="1">
+        <v>57494</v>
+      </c>
       <c r="D202" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
@@ -4371,9 +4518,12 @@
       <c r="B203" s="1">
         <v>60027</v>
       </c>
+      <c r="C203" s="1">
+        <v>59997</v>
+      </c>
       <c r="D203" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4.9977510120445795E-4</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
@@ -4383,9 +4533,12 @@
       <c r="B204" s="1">
         <v>58025</v>
       </c>
+      <c r="C204" s="1">
+        <v>57977</v>
+      </c>
       <c r="D204" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>8.2722964239551912E-4</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
@@ -4395,9 +4548,12 @@
       <c r="B205" s="1">
         <v>60776</v>
       </c>
+      <c r="C205" s="1">
+        <v>60776</v>
+      </c>
       <c r="D205" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
@@ -4407,9 +4563,12 @@
       <c r="B206" s="1">
         <v>58884</v>
       </c>
+      <c r="C206" s="1">
+        <v>58816</v>
+      </c>
       <c r="D206" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.1548128523877453E-3</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
@@ -4419,9 +4578,12 @@
       <c r="B207" s="1">
         <v>60011</v>
       </c>
+      <c r="C207" s="1">
+        <v>59830</v>
+      </c>
       <c r="D207" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.0161137124860441E-3</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
@@ -4431,9 +4593,12 @@
       <c r="B208" s="1">
         <v>58132</v>
       </c>
+      <c r="C208" s="1">
+        <v>58132</v>
+      </c>
       <c r="D208" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
@@ -4443,9 +4608,12 @@
       <c r="B209" s="1">
         <v>59064</v>
       </c>
+      <c r="C209" s="1">
+        <v>58944</v>
+      </c>
       <c r="D209" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.0316944331572532E-3</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
@@ -4455,9 +4623,12 @@
       <c r="B210" s="1">
         <v>58975</v>
       </c>
+      <c r="C210" s="1">
+        <v>58856</v>
+      </c>
       <c r="D210" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2.0178041543026707E-3</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
@@ -4467,9 +4638,12 @@
       <c r="B211" s="1">
         <v>60603</v>
       </c>
+      <c r="C211" s="1">
+        <v>60574</v>
+      </c>
       <c r="D211" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4.7852416547035625E-4</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
@@ -4480,11 +4654,11 @@
         <v>56693</v>
       </c>
       <c r="C212">
-        <v>56374</v>
+        <v>56572</v>
       </c>
       <c r="D212" s="2">
         <f t="shared" si="3"/>
-        <v>5.6267969590602018E-3</v>
+        <v>2.1343022948159384E-3</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4495,11 +4669,11 @@
         <v>58318</v>
       </c>
       <c r="C213">
-        <v>57962</v>
+        <v>58064</v>
       </c>
       <c r="D213" s="2">
         <f t="shared" si="3"/>
-        <v>6.1044617442299115E-3</v>
+        <v>4.3554305703213418E-3</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
@@ -4510,11 +4684,11 @@
         <v>56553</v>
       </c>
       <c r="C214">
-        <v>56291</v>
+        <v>55722</v>
       </c>
       <c r="D214" s="2">
         <f t="shared" si="3"/>
-        <v>4.6328223082771911E-3</v>
+        <v>1.4694180680070022E-2</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
@@ -4525,11 +4699,11 @@
         <v>56863</v>
       </c>
       <c r="C215">
-        <v>56563</v>
+        <v>58451</v>
       </c>
       <c r="D215" s="2">
         <f t="shared" si="3"/>
-        <v>5.2758384186553644E-3</v>
+        <v>-2.7926771362749063E-2</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>